<commit_message>
Update the code for DVT Led HW Change
</commit_message>
<xml_diff>
--- a/R1_test_command_list_tag1.7PTE.xlsx
+++ b/R1_test_command_list_tag1.7PTE.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="commands_list" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="264">
   <si>
     <t>./inventory.sh</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -72,12 +72,6 @@
     <t>#</t>
   </si>
   <si>
-    <t>ACTION_b</t>
-  </si>
-  <si>
-    <t>ACTION_g</t>
-  </si>
-  <si>
     <t>ACTION_r</t>
   </si>
   <si>
@@ -111,9 +105,6 @@
     <t>Lantern_W3_r</t>
   </si>
   <si>
-    <t>Lantern_b</t>
-  </si>
-  <si>
     <t>Lantern_g</t>
   </si>
   <si>
@@ -192,36 +183,21 @@
     <t>Lantern_r</t>
   </si>
   <si>
-    <t>PLAYPAUSE_b</t>
-  </si>
-  <si>
     <t>PLAYPAUSE_g</t>
   </si>
   <si>
     <t>PLAYPAUSE_r</t>
   </si>
   <si>
-    <t>USB_b</t>
-  </si>
-  <si>
-    <t>USB_g</t>
-  </si>
-  <si>
     <t>USB_r</t>
   </si>
   <si>
-    <t>VOL+_b</t>
-  </si>
-  <si>
     <t>VOL+_g</t>
   </si>
   <si>
     <t>VOL+_r</t>
   </si>
   <si>
-    <t>VOL-_b</t>
-  </si>
-  <si>
     <t>VOL-_g</t>
   </si>
   <si>
@@ -231,25 +207,7 @@
     <t>Lantern White</t>
   </si>
   <si>
-    <t>USB</t>
-  </si>
-  <si>
-    <t>Lantern Key</t>
-  </si>
-  <si>
-    <t>Action Key</t>
-  </si>
-  <si>
     <t>Connect Key</t>
-  </si>
-  <si>
-    <t>Pause Key</t>
-  </si>
-  <si>
-    <t>Volume+ Key</t>
-  </si>
-  <si>
-    <t>Volume- Key</t>
   </si>
   <si>
     <t>Lantern Red</t>
@@ -1111,6 +1069,34 @@
   </si>
   <si>
     <t>New add command</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Volume+ Key</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Volume- Key</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>USB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pause Key</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lantern Key</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Action Key</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ACTION_g</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1318,7 +1304,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1398,9 +1384,21 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1415,15 +1413,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1731,8 +1720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1750,7 +1739,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="15" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="B1" s="15" t="s">
         <v>16</v>
@@ -1765,63 +1754,63 @@
         <v>15</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="G1" s="16" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="H1" s="16" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="41.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="37" t="s">
-        <v>100</v>
+      <c r="A2" s="33" t="s">
+        <v>86</v>
       </c>
       <c r="B2" s="25">
         <v>1</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="E2" s="17" t="s">
         <v>10</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>241</v>
+        <v>227</v>
       </c>
       <c r="G2" s="18"/>
       <c r="H2" s="10" t="s">
-        <v>183</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="99.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="38"/>
+      <c r="A3" s="34"/>
       <c r="B3" s="25">
         <v>2</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="D3" s="24" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>264</v>
+        <v>250</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>241</v>
+        <v>227</v>
       </c>
       <c r="G3" s="18" t="s">
-        <v>263</v>
+        <v>249</v>
       </c>
       <c r="H3" s="28"/>
     </row>
     <row r="4" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="38"/>
+      <c r="A4" s="34"/>
       <c r="B4" s="25">
         <v>3</v>
       </c>
@@ -1829,21 +1818,21 @@
         <v>2</v>
       </c>
       <c r="D4" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="E4" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="E4" s="18" t="s">
-        <v>96</v>
-      </c>
       <c r="F4" s="18" t="s">
-        <v>241</v>
+        <v>227</v>
       </c>
       <c r="G4" s="18" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="H4" s="28"/>
     </row>
     <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="38"/>
+      <c r="A5" s="34"/>
       <c r="B5" s="25">
         <v>4</v>
       </c>
@@ -1851,43 +1840,43 @@
         <v>3</v>
       </c>
       <c r="D5" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="E5" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="E5" s="18" t="s">
-        <v>97</v>
-      </c>
       <c r="F5" s="18" t="s">
-        <v>241</v>
+        <v>227</v>
       </c>
       <c r="G5" s="18" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="H5" s="28"/>
     </row>
     <row r="6" spans="1:8" ht="46.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="38"/>
+      <c r="A6" s="34"/>
       <c r="B6" s="25">
         <v>5</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="E6" s="18" t="s">
         <v>7</v>
       </c>
       <c r="F6" s="18" t="s">
-        <v>241</v>
+        <v>227</v>
       </c>
       <c r="G6" s="18" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="H6" s="28"/>
     </row>
     <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="38"/>
+      <c r="A7" s="34"/>
       <c r="B7" s="25">
         <v>6</v>
       </c>
@@ -1895,57 +1884,57 @@
         <v>4</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="E7" s="17" t="s">
         <v>12</v>
       </c>
       <c r="F7" s="18" t="s">
-        <v>241</v>
+        <v>227</v>
       </c>
       <c r="G7" s="18"/>
       <c r="H7" s="28"/>
     </row>
     <row r="8" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="38"/>
+      <c r="A8" s="34"/>
       <c r="B8" s="25"/>
       <c r="C8" s="20"/>
       <c r="D8" s="18" t="s">
-        <v>255</v>
+        <v>241</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>244</v>
+        <v>230</v>
       </c>
       <c r="F8" s="18" t="s">
-        <v>245</v>
+        <v>231</v>
       </c>
       <c r="G8" s="18"/>
       <c r="H8" s="28"/>
     </row>
     <row r="9" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="38"/>
+      <c r="A9" s="34"/>
       <c r="B9" s="25">
         <v>7</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>246</v>
+        <v>232</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>243</v>
+        <v>229</v>
       </c>
       <c r="H9" s="28"/>
     </row>
     <row r="10" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="38"/>
+      <c r="A10" s="34"/>
       <c r="B10" s="25">
         <v>8</v>
       </c>
@@ -1953,131 +1942,131 @@
         <v>0</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="E10" s="18" t="s">
         <v>6</v>
       </c>
       <c r="F10" s="18" t="s">
-        <v>242</v>
+        <v>228</v>
       </c>
       <c r="G10" s="18" t="s">
-        <v>192</v>
+        <v>178</v>
       </c>
       <c r="H10" s="28"/>
     </row>
     <row r="11" spans="1:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="38"/>
+      <c r="A11" s="34"/>
       <c r="B11" s="25">
         <v>9</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="E11" s="17" t="s">
         <v>11</v>
       </c>
       <c r="F11" s="18" t="s">
-        <v>242</v>
+        <v>228</v>
       </c>
       <c r="G11" s="18" t="s">
-        <v>193</v>
+        <v>179</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>224</v>
+        <v>210</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="38"/>
+      <c r="A12" s="34"/>
       <c r="B12" s="25">
         <v>10</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>195</v>
+        <v>181</v>
       </c>
       <c r="F12" s="18" t="s">
-        <v>242</v>
+        <v>228</v>
       </c>
       <c r="G12" s="29" t="s">
-        <v>194</v>
+        <v>180</v>
       </c>
       <c r="H12" s="28"/>
     </row>
     <row r="13" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="38"/>
+      <c r="A13" s="34"/>
       <c r="B13" s="25">
         <v>11</v>
       </c>
       <c r="C13" s="20" t="s">
-        <v>197</v>
+        <v>183</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>196</v>
+        <v>182</v>
       </c>
       <c r="E13" s="18" t="s">
         <v>9</v>
       </c>
       <c r="F13" s="18" t="s">
-        <v>242</v>
+        <v>228</v>
       </c>
       <c r="G13" s="18"/>
       <c r="H13" s="28"/>
     </row>
     <row r="14" spans="1:8" ht="46.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="38"/>
+      <c r="A14" s="34"/>
       <c r="B14" s="25">
         <v>12</v>
       </c>
       <c r="C14" s="20" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>198</v>
+        <v>184</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="F14" s="18" t="s">
-        <v>242</v>
+        <v>228</v>
       </c>
       <c r="G14" s="18"/>
       <c r="H14" s="10" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="46.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="38"/>
+      <c r="A15" s="34"/>
       <c r="B15" s="25">
         <v>13</v>
       </c>
       <c r="C15" s="20" t="s">
-        <v>232</v>
+        <v>218</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>233</v>
+        <v>219</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>186</v>
+        <v>172</v>
       </c>
       <c r="F15" s="18" t="s">
-        <v>242</v>
+        <v>228</v>
       </c>
       <c r="G15" s="18"/>
       <c r="H15" s="10" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="38"/>
+      <c r="A16" s="34"/>
       <c r="B16" s="25">
         <v>14</v>
       </c>
@@ -2085,794 +2074,794 @@
         <v>1</v>
       </c>
       <c r="D16" s="24" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="E16" s="18" t="s">
         <v>5</v>
       </c>
       <c r="F16" s="18" t="s">
-        <v>241</v>
+        <v>227</v>
       </c>
       <c r="G16" s="18" t="s">
-        <v>141</v>
+        <v>127</v>
       </c>
       <c r="H16" s="28"/>
     </row>
     <row r="17" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="38"/>
+      <c r="A17" s="34"/>
       <c r="B17" s="25">
         <v>15</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="D17" s="24" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
       <c r="E17" s="17" t="s">
         <v>8</v>
       </c>
       <c r="F17" s="30" t="s">
-        <v>262</v>
+        <v>248</v>
       </c>
       <c r="G17" s="18" t="s">
-        <v>261</v>
+        <v>247</v>
       </c>
       <c r="H17" s="28"/>
     </row>
     <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="38"/>
+      <c r="A18" s="34"/>
       <c r="B18" s="25">
         <v>16</v>
       </c>
       <c r="C18" s="20" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
       <c r="E18" s="17" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="F18" s="18" t="s">
-        <v>242</v>
+        <v>228</v>
       </c>
       <c r="G18" s="18" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="H18" s="28"/>
     </row>
     <row r="19" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="38"/>
+      <c r="A19" s="34"/>
       <c r="B19" s="25">
         <v>17</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="D19" s="18"/>
       <c r="E19" s="17" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="F19" s="30" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
       <c r="G19" s="18"/>
       <c r="H19" s="12"/>
     </row>
     <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="38"/>
+      <c r="A20" s="34"/>
       <c r="B20" s="25">
         <v>18</v>
       </c>
       <c r="C20" s="20" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
       <c r="E20" s="23" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="F20" s="18"/>
       <c r="G20" s="18" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="H20" s="28"/>
     </row>
     <row r="21" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="38"/>
+      <c r="A21" s="34"/>
       <c r="B21" s="25">
         <v>19</v>
       </c>
       <c r="C21" s="20" t="s">
-        <v>150</v>
+        <v>136</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
       <c r="E21" s="23" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="F21" s="18"/>
       <c r="G21" s="18" t="s">
-        <v>148</v>
+        <v>134</v>
       </c>
       <c r="H21" s="28"/>
     </row>
     <row r="22" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="38"/>
+      <c r="A22" s="34"/>
       <c r="B22" s="25">
         <v>20</v>
       </c>
       <c r="C22" s="20" t="s">
-        <v>200</v>
+        <v>186</v>
       </c>
       <c r="D22" s="23" t="s">
-        <v>253</v>
+        <v>239</v>
       </c>
       <c r="E22" s="17" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="F22" s="23" t="s">
-        <v>241</v>
+        <v>227</v>
       </c>
       <c r="G22" s="18" t="s">
-        <v>254</v>
+        <v>240</v>
       </c>
       <c r="H22" s="10" t="s">
-        <v>225</v>
+        <v>211</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="38"/>
+      <c r="A23" s="34"/>
       <c r="B23" s="25">
         <v>21</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>151</v>
+        <v>137</v>
       </c>
       <c r="D23" s="23" t="s">
-        <v>249</v>
+        <v>235</v>
       </c>
       <c r="E23" s="23" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="F23" s="23" t="s">
-        <v>245</v>
+        <v>231</v>
       </c>
       <c r="G23" s="18" t="s">
-        <v>252</v>
+        <v>238</v>
       </c>
       <c r="H23" s="28"/>
     </row>
     <row r="24" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="38"/>
+      <c r="A24" s="34"/>
       <c r="B24" s="25">
         <v>22</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
       <c r="D24" s="23" t="s">
-        <v>250</v>
+        <v>236</v>
       </c>
       <c r="E24" s="23" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="F24" s="18" t="s">
-        <v>245</v>
+        <v>231</v>
       </c>
       <c r="G24" s="18" t="s">
-        <v>251</v>
+        <v>237</v>
       </c>
       <c r="H24" s="28"/>
     </row>
     <row r="25" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="38"/>
+      <c r="A25" s="34"/>
       <c r="B25" s="25">
         <v>23</v>
       </c>
       <c r="C25" s="20" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
       <c r="D25" s="23" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="E25" s="23" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="F25" s="18" t="s">
-        <v>242</v>
+        <v>228</v>
       </c>
       <c r="G25" s="18" t="s">
-        <v>154</v>
+        <v>140</v>
       </c>
       <c r="H25" s="12"/>
     </row>
     <row r="26" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="38"/>
+      <c r="A26" s="34"/>
       <c r="B26" s="25">
         <v>24</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="D26" s="23" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="E26" s="23" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="F26" s="18" t="s">
-        <v>242</v>
+        <v>228</v>
       </c>
       <c r="G26" s="18" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="H26" s="12"/>
     </row>
     <row r="27" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="38"/>
+      <c r="A27" s="34"/>
       <c r="B27" s="25">
         <v>25</v>
       </c>
       <c r="C27" s="20" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
       <c r="D27" s="23" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="E27" s="23" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="F27" s="18" t="s">
-        <v>242</v>
+        <v>228</v>
       </c>
       <c r="G27" s="18" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="H27" s="12"/>
     </row>
     <row r="28" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="38"/>
+      <c r="A28" s="34"/>
       <c r="B28" s="25">
         <v>26</v>
       </c>
       <c r="C28" s="20" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="D28" s="23" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="E28" s="23" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="F28" s="18" t="s">
-        <v>242</v>
+        <v>228</v>
       </c>
       <c r="G28" s="18" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="H28" s="12"/>
     </row>
     <row r="29" spans="1:8" ht="52.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="38"/>
+      <c r="A29" s="34"/>
       <c r="B29" s="25">
         <v>27</v>
       </c>
       <c r="C29" s="20" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
       <c r="D29" s="23" t="s">
-        <v>165</v>
+        <v>151</v>
       </c>
       <c r="E29" s="23" t="s">
-        <v>182</v>
+        <v>168</v>
       </c>
       <c r="F29" s="18" t="s">
-        <v>241</v>
+        <v>227</v>
       </c>
       <c r="G29" s="18" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
       <c r="H29" s="11" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="38"/>
+      <c r="A30" s="34"/>
       <c r="B30" s="25">
         <v>28</v>
       </c>
       <c r="C30" s="23" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="D30" s="23"/>
       <c r="E30" s="23" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="F30" s="18" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="G30" s="18"/>
       <c r="H30" s="11" t="s">
-        <v>190</v>
+        <v>176</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="38"/>
+      <c r="A31" s="34"/>
       <c r="B31" s="25">
         <v>29</v>
       </c>
       <c r="C31" s="20" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="D31" s="23" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
       <c r="E31" s="23" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="F31" s="18" t="s">
-        <v>245</v>
+        <v>231</v>
       </c>
       <c r="G31" s="18" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="H31" s="28"/>
     </row>
     <row r="32" spans="1:8" ht="58.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="38"/>
+      <c r="A32" s="34"/>
       <c r="B32" s="25">
         <v>31</v>
       </c>
       <c r="C32" s="20" t="s">
-        <v>216</v>
+        <v>202</v>
       </c>
       <c r="D32" s="23" t="s">
-        <v>214</v>
+        <v>200</v>
       </c>
       <c r="E32" s="23" t="s">
-        <v>187</v>
+        <v>173</v>
       </c>
       <c r="F32" s="27" t="s">
-        <v>241</v>
+        <v>227</v>
       </c>
       <c r="G32" s="18" t="s">
-        <v>215</v>
+        <v>201</v>
       </c>
       <c r="H32" s="10" t="s">
-        <v>226</v>
+        <v>212</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="76.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="38"/>
+      <c r="A33" s="34"/>
       <c r="B33" s="25">
         <v>32</v>
       </c>
       <c r="C33" s="20" t="s">
-        <v>217</v>
+        <v>203</v>
       </c>
       <c r="D33" s="23" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
       <c r="E33" s="23" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
       <c r="F33" s="27" t="s">
-        <v>241</v>
+        <v>227</v>
       </c>
       <c r="G33" s="18" t="s">
-        <v>213</v>
+        <v>199</v>
       </c>
       <c r="H33" s="10" t="s">
-        <v>226</v>
+        <v>212</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="38"/>
+      <c r="A34" s="34"/>
       <c r="B34" s="25">
         <v>33</v>
       </c>
       <c r="C34" s="20" t="s">
-        <v>170</v>
+        <v>156</v>
       </c>
       <c r="D34" s="23" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="E34" s="23" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="F34" s="18" t="s">
-        <v>245</v>
+        <v>231</v>
       </c>
       <c r="G34" s="18" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="H34" s="28"/>
     </row>
     <row r="35" spans="1:8" ht="48.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="38"/>
+      <c r="A35" s="34"/>
       <c r="B35" s="25">
         <v>34</v>
       </c>
       <c r="C35" s="30" t="s">
-        <v>181</v>
+        <v>167</v>
       </c>
       <c r="D35" s="23" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
       <c r="E35" s="23" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="F35" s="30" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="G35" s="18" t="s">
-        <v>258</v>
+        <v>244</v>
       </c>
       <c r="H35" s="28"/>
     </row>
     <row r="36" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="38"/>
+      <c r="A36" s="34"/>
       <c r="B36" s="25">
         <v>35</v>
       </c>
       <c r="C36" s="23" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="D36" s="23"/>
       <c r="E36" s="23" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="F36" s="30" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
       <c r="G36" s="18"/>
       <c r="H36" s="12"/>
     </row>
     <row r="37" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="38"/>
+      <c r="A37" s="34"/>
       <c r="B37" s="25">
         <v>36</v>
       </c>
       <c r="C37" s="20" t="s">
-        <v>204</v>
+        <v>190</v>
       </c>
       <c r="D37" s="23" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
       <c r="E37" s="23" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="F37" s="18" t="s">
-        <v>242</v>
+        <v>228</v>
       </c>
       <c r="G37" s="27" t="s">
-        <v>203</v>
+        <v>189</v>
       </c>
       <c r="H37" s="28"/>
     </row>
     <row r="38" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A38" s="38"/>
+      <c r="A38" s="34"/>
       <c r="B38" s="25">
         <v>37</v>
       </c>
       <c r="C38" s="20" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="D38" s="23" t="s">
-        <v>212</v>
+        <v>198</v>
       </c>
       <c r="E38" s="23" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="F38" s="18" t="s">
-        <v>242</v>
+        <v>228</v>
       </c>
       <c r="G38" s="27" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="H38" s="28"/>
     </row>
     <row r="39" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A39" s="38"/>
+      <c r="A39" s="34"/>
       <c r="B39" s="25">
         <v>38</v>
       </c>
       <c r="C39" s="23" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D39" s="23"/>
       <c r="E39" s="23" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="F39" s="30" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
       <c r="G39" s="18"/>
       <c r="H39" s="12"/>
     </row>
     <row r="40" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A40" s="38"/>
+      <c r="A40" s="34"/>
       <c r="B40" s="25">
         <v>39</v>
       </c>
       <c r="C40" s="20" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="D40" s="23" t="s">
-        <v>239</v>
+        <v>225</v>
       </c>
       <c r="E40" s="23" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="F40" s="18" t="s">
-        <v>245</v>
+        <v>231</v>
       </c>
       <c r="G40" s="18" t="s">
-        <v>240</v>
+        <v>226</v>
       </c>
       <c r="H40" s="12"/>
     </row>
     <row r="41" spans="1:8" ht="88.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A41" s="38"/>
+      <c r="A41" s="34"/>
       <c r="B41" s="25">
         <v>40</v>
       </c>
       <c r="C41" s="20" t="s">
-        <v>247</v>
+        <v>233</v>
       </c>
       <c r="D41" s="23" t="s">
-        <v>211</v>
+        <v>197</v>
       </c>
       <c r="E41" s="23" t="s">
-        <v>180</v>
+        <v>166</v>
       </c>
       <c r="F41" s="19" t="s">
-        <v>248</v>
+        <v>234</v>
       </c>
       <c r="G41" s="18" t="s">
-        <v>235</v>
+        <v>221</v>
       </c>
       <c r="H41" s="12"/>
     </row>
     <row r="42" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A42" s="38"/>
+      <c r="A42" s="34"/>
       <c r="B42" s="25">
         <v>41</v>
       </c>
       <c r="C42" s="21" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="D42" s="23"/>
       <c r="E42" s="23" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="F42" s="30" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
       <c r="G42" s="18"/>
       <c r="H42" s="11" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A43" s="38"/>
+      <c r="A43" s="34"/>
       <c r="B43" s="25">
         <v>45</v>
       </c>
       <c r="C43" s="20" t="s">
-        <v>256</v>
+        <v>242</v>
       </c>
       <c r="D43" s="23" t="s">
-        <v>227</v>
+        <v>213</v>
       </c>
       <c r="E43" s="23" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="F43" s="18" t="s">
-        <v>245</v>
+        <v>231</v>
       </c>
       <c r="G43" s="18"/>
       <c r="H43" s="28"/>
     </row>
     <row r="44" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A44" s="38"/>
+      <c r="A44" s="34"/>
       <c r="B44" s="25">
         <v>46</v>
       </c>
       <c r="C44" s="20" t="s">
-        <v>257</v>
+        <v>243</v>
       </c>
       <c r="D44" s="23" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
       <c r="E44" s="23" t="s">
-        <v>222</v>
+        <v>208</v>
       </c>
       <c r="F44" s="18" t="s">
-        <v>245</v>
+        <v>231</v>
       </c>
       <c r="G44" s="18"/>
       <c r="H44" s="28"/>
     </row>
     <row r="45" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A45" s="38"/>
+      <c r="A45" s="34"/>
       <c r="B45" s="25">
         <v>47</v>
       </c>
       <c r="C45" s="20" t="s">
-        <v>209</v>
+        <v>195</v>
       </c>
       <c r="D45" s="23" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
       <c r="E45" s="23" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="F45" s="18" t="s">
-        <v>242</v>
+        <v>228</v>
       </c>
       <c r="G45" s="27" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
       <c r="H45" s="28"/>
     </row>
     <row r="46" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A46" s="38"/>
+      <c r="A46" s="34"/>
       <c r="B46" s="25">
         <v>48</v>
       </c>
       <c r="C46" s="20" t="s">
-        <v>210</v>
+        <v>196</v>
       </c>
       <c r="D46" s="23" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
       <c r="E46" s="23" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="F46" s="18" t="s">
-        <v>242</v>
+        <v>228</v>
       </c>
       <c r="G46" s="27" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
       <c r="H46" s="28"/>
     </row>
     <row r="47" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A47" s="38"/>
+      <c r="A47" s="34"/>
       <c r="B47" s="25">
         <v>49</v>
       </c>
       <c r="C47" s="19" t="s">
-        <v>228</v>
+        <v>214</v>
       </c>
       <c r="D47" s="24"/>
       <c r="E47" s="23" t="s">
-        <v>266</v>
+        <v>252</v>
       </c>
       <c r="F47" s="18" t="s">
-        <v>270</v>
+        <v>256</v>
       </c>
       <c r="G47" s="27"/>
       <c r="H47" s="28"/>
     </row>
     <row r="48" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A48" s="38"/>
+      <c r="A48" s="34"/>
       <c r="B48" s="25">
         <v>50</v>
       </c>
       <c r="C48" s="19" t="s">
-        <v>229</v>
+        <v>215</v>
       </c>
       <c r="D48" s="24"/>
       <c r="E48" s="23" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
       <c r="F48" s="18" t="s">
-        <v>270</v>
+        <v>256</v>
       </c>
       <c r="G48" s="27"/>
       <c r="H48" s="28"/>
     </row>
     <row r="49" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A49" s="38"/>
+      <c r="A49" s="34"/>
       <c r="B49" s="25">
         <v>51</v>
       </c>
       <c r="C49" s="19" t="s">
-        <v>230</v>
+        <v>216</v>
       </c>
       <c r="D49" s="24"/>
       <c r="E49" s="23" t="s">
-        <v>268</v>
+        <v>254</v>
       </c>
       <c r="F49" s="18" t="s">
-        <v>270</v>
+        <v>256</v>
       </c>
       <c r="G49" s="27"/>
       <c r="H49" s="28"/>
     </row>
     <row r="50" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A50" s="38"/>
+      <c r="A50" s="34"/>
       <c r="B50" s="25">
         <v>52</v>
       </c>
       <c r="C50" s="19" t="s">
-        <v>265</v>
+        <v>251</v>
       </c>
       <c r="D50" s="24"/>
       <c r="E50" s="23" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="F50" s="18" t="s">
-        <v>270</v>
+        <v>256</v>
       </c>
       <c r="G50" s="27"/>
       <c r="H50" s="28"/>
     </row>
     <row r="51" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A51" s="39"/>
+      <c r="A51" s="35"/>
       <c r="B51" s="25">
         <v>53</v>
       </c>
       <c r="C51" s="24"/>
       <c r="D51" s="24" t="s">
-        <v>236</v>
+        <v>222</v>
       </c>
       <c r="E51" s="23"/>
       <c r="F51" s="18"/>
       <c r="G51" s="27" t="s">
-        <v>237</v>
+        <v>223</v>
       </c>
       <c r="H51" s="28"/>
     </row>
     <row r="52" spans="1:8" ht="57.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A52" s="31" t="s">
-        <v>99</v>
+      <c r="A52" s="32" t="s">
+        <v>85</v>
       </c>
       <c r="B52" s="26">
         <v>1</v>
       </c>
       <c r="C52" s="24" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="D52" s="24" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
       <c r="E52" s="24" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
       <c r="F52" s="18" t="s">
-        <v>245</v>
+        <v>231</v>
       </c>
       <c r="G52" s="18" t="s">
-        <v>260</v>
+        <v>246</v>
       </c>
       <c r="H52" s="28"/>
     </row>
     <row r="53" spans="1:8" ht="51.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A53" s="31"/>
+      <c r="A53" s="32"/>
       <c r="B53" s="26">
         <v>2</v>
       </c>
       <c r="C53" s="24" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="D53" s="24" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
       <c r="E53" s="24" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
       <c r="F53" s="18" t="s">
-        <v>245</v>
+        <v>231</v>
       </c>
       <c r="G53" s="18" t="s">
-        <v>238</v>
+        <v>224</v>
       </c>
       <c r="H53" s="28"/>
     </row>
@@ -2892,17 +2881,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C54"/>
+  <dimension ref="A1:C47"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="13.75" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.75" style="3" customWidth="1"/>
-    <col min="3" max="3" width="31.875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="39.375" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.75" style="2" customWidth="1"/>
     <col min="5" max="5" width="31.625" style="2" customWidth="1"/>
     <col min="6" max="6" width="14.875" style="2" bestFit="1" customWidth="1"/>
@@ -2911,397 +2900,354 @@
     <col min="9" max="16384" width="9.125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A1" s="36" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A1" s="40" t="s">
+        <v>262</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A2" s="40"/>
+      <c r="B2" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A3" s="40" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A2" s="36"/>
-      <c r="B2" s="7" t="s">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A4" s="40"/>
+      <c r="B4" s="7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A3" s="36"/>
-      <c r="B3" s="6" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A5" s="40"/>
+      <c r="B5" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A4" s="36" t="s">
-        <v>73</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A5" s="36"/>
-      <c r="B5" s="7" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A6" s="40" t="s">
+        <v>261</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A7" s="40"/>
+      <c r="B7" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A8" s="40" t="s">
+        <v>260</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A9" s="40"/>
+      <c r="B9" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A10" s="31" t="s">
+        <v>259</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A11" s="39" t="s">
+        <v>257</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A12" s="39"/>
+      <c r="B12" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A13" s="39" t="s">
+        <v>258</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A14" s="39"/>
+      <c r="B14" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A15" s="39" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A6" s="36"/>
-      <c r="B6" s="6" t="s">
+      <c r="C15" s="36" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A16" s="39"/>
+      <c r="B16" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A7" s="36" t="s">
-        <v>71</v>
-      </c>
-      <c r="B7" s="8" t="s">
+      <c r="C16" s="37"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A17" s="39"/>
+      <c r="B17" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="37"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A18" s="39"/>
+      <c r="B18" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="37"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A19" s="39"/>
+      <c r="B19" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="37"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A20" s="39"/>
+      <c r="B20" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="37"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A21" s="39"/>
+      <c r="B21" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="37"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A22" s="39"/>
+      <c r="B22" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" s="37"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A23" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="37"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A24" s="39"/>
+      <c r="B24" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" s="37"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A25" s="39"/>
+      <c r="B25" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" s="37"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A26" s="39"/>
+      <c r="B26" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" s="37"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A27" s="39"/>
+      <c r="B27" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C27" s="37"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A28" s="39"/>
+      <c r="B28" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C28" s="37"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A29" s="39"/>
+      <c r="B29" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C29" s="37"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A30" s="39"/>
+      <c r="B30" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C30" s="37"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A31" s="39" t="s">
+        <v>64</v>
+      </c>
+      <c r="B31" s="7" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A8" s="36"/>
-      <c r="B8" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A9" s="36"/>
-      <c r="B9" s="6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A10" s="36" t="s">
-        <v>74</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A11" s="36"/>
-      <c r="B11" s="7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A12" s="36"/>
-      <c r="B12" s="6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A13" s="36" t="s">
-        <v>70</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A14" s="36"/>
-      <c r="B14" s="7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A15" s="36"/>
-      <c r="B15" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A16" s="35" t="s">
-        <v>75</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A17" s="35"/>
-      <c r="B17" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A18" s="35"/>
-      <c r="B18" s="6" t="s">
+      <c r="C31" s="37"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A32" s="39"/>
+      <c r="B32" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C32" s="37"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A33" s="39"/>
+      <c r="B33" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C33" s="37"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A34" s="39"/>
+      <c r="B34" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C34" s="37"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A35" s="39"/>
+      <c r="B35" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C35" s="37"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A36" s="39"/>
+      <c r="B36" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C36" s="37"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A37" s="39"/>
+      <c r="B37" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C37" s="37"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A38" s="39"/>
+      <c r="B38" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C38" s="37"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A39" s="39" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A19" s="35" t="s">
-        <v>76</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A20" s="35"/>
-      <c r="B20" s="7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A21" s="35"/>
-      <c r="B21" s="6" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A22" s="35" t="s">
-        <v>69</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C22" s="32" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A23" s="35"/>
-      <c r="B23" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C23" s="33"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A24" s="35"/>
-      <c r="B24" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C24" s="33"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A25" s="35"/>
-      <c r="B25" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C25" s="33"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A26" s="35"/>
-      <c r="B26" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C26" s="33"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A27" s="35"/>
-      <c r="B27" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C27" s="33"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A28" s="35"/>
-      <c r="B28" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C28" s="33"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A29" s="35"/>
-      <c r="B29" s="5" t="s">
+      <c r="B39" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C29" s="33"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A30" s="35" t="s">
-        <v>77</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C30" s="33"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A31" s="35"/>
-      <c r="B31" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C31" s="33"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A32" s="35"/>
-      <c r="B32" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C32" s="33"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A33" s="35"/>
-      <c r="B33" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C33" s="33"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A34" s="35"/>
-      <c r="B34" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C34" s="33"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A35" s="35"/>
-      <c r="B35" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C35" s="33"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A36" s="35"/>
-      <c r="B36" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C36" s="33"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A37" s="35"/>
-      <c r="B37" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C37" s="33"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A38" s="35" t="s">
-        <v>78</v>
-      </c>
-      <c r="B38" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C38" s="33"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A39" s="35"/>
-      <c r="B39" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C39" s="33"/>
+      <c r="C39" s="37"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A40" s="35"/>
-      <c r="B40" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C40" s="33"/>
+      <c r="A40" s="39"/>
+      <c r="B40" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C40" s="37"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A41" s="35"/>
-      <c r="B41" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C41" s="33"/>
+      <c r="A41" s="39"/>
+      <c r="B41" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C41" s="37"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A42" s="35"/>
-      <c r="B42" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="C42" s="33"/>
+      <c r="A42" s="39"/>
+      <c r="B42" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C42" s="37"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A43" s="35"/>
-      <c r="B43" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C43" s="33"/>
+      <c r="A43" s="39"/>
+      <c r="B43" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C43" s="37"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A44" s="35"/>
-      <c r="B44" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="C44" s="33"/>
+      <c r="A44" s="39"/>
+      <c r="B44" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C44" s="37"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A45" s="35"/>
-      <c r="B45" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="C45" s="33"/>
+      <c r="A45" s="39"/>
+      <c r="B45" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C45" s="37"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A46" s="35" t="s">
-        <v>79</v>
-      </c>
+      <c r="A46" s="39"/>
       <c r="B46" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C46" s="33"/>
+        <v>50</v>
+      </c>
+      <c r="C46" s="38"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A47" s="35"/>
-      <c r="B47" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C47" s="33"/>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A48" s="35"/>
-      <c r="B48" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C48" s="33"/>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A49" s="35"/>
-      <c r="B49" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="C49" s="33"/>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A50" s="35"/>
-      <c r="B50" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="C50" s="33"/>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A51" s="35"/>
-      <c r="B51" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C51" s="33"/>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A52" s="35"/>
-      <c r="B52" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C52" s="33"/>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A53" s="35"/>
-      <c r="B53" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="C53" s="34"/>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A54" s="9"/>
+      <c r="A47" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="C22:C53"/>
-    <mergeCell ref="A22:A29"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="A19:A21"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="A30:A37"/>
-    <mergeCell ref="A38:A45"/>
-    <mergeCell ref="A46:A53"/>
-    <mergeCell ref="A16:A18"/>
+  <mergeCells count="11">
+    <mergeCell ref="C15:C46"/>
+    <mergeCell ref="A15:A22"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A23:A30"/>
+    <mergeCell ref="A31:A38"/>
+    <mergeCell ref="A39:A46"/>
+    <mergeCell ref="A11:A12"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add mute key to R1_test_command_list_tag1.7PTE.xlsx
</commit_message>
<xml_diff>
--- a/R1_test_command_list_tag1.7PTE.xlsx
+++ b/R1_test_command_list_tag1.7PTE.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="269">
   <si>
     <t>./inventory.sh</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -196,12 +196,6 @@
   </si>
   <si>
     <t>VOL+_r</t>
-  </si>
-  <si>
-    <t>VOL-_g</t>
-  </si>
-  <si>
-    <t>VOL-_r</t>
   </si>
   <si>
     <t>Lantern White</t>
@@ -1097,6 +1091,34 @@
   </si>
   <si>
     <t>ACTION_g</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VOL-_r</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mute_r</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mute Key</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VOL-_g</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mute_g</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Only White/Red for Mute key</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Only White for Mute key</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1240,7 +1262,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -1300,11 +1322,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1413,6 +1455,18 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1739,7 +1793,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="15" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B1" s="15" t="s">
         <v>16</v>
@@ -1754,37 +1808,37 @@
         <v>15</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G1" s="16" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H1" s="16" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="41.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="33" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B2" s="25">
         <v>1</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E2" s="17" t="s">
         <v>10</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G2" s="18"/>
       <c r="H2" s="10" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="99.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1793,19 +1847,19 @@
         <v>2</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D3" s="24" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G3" s="18" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="H3" s="28"/>
     </row>
@@ -1818,16 +1872,16 @@
         <v>2</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F4" s="18" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G4" s="18" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H4" s="28"/>
     </row>
@@ -1840,16 +1894,16 @@
         <v>3</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F5" s="18" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G5" s="18" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="H5" s="28"/>
     </row>
@@ -1859,19 +1913,19 @@
         <v>5</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E6" s="18" t="s">
         <v>7</v>
       </c>
       <c r="F6" s="18" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G6" s="18" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="H6" s="28"/>
     </row>
@@ -1884,13 +1938,13 @@
         <v>4</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E7" s="17" t="s">
         <v>12</v>
       </c>
       <c r="F7" s="18" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G7" s="18"/>
       <c r="H7" s="28"/>
@@ -1900,13 +1954,13 @@
       <c r="B8" s="25"/>
       <c r="C8" s="20"/>
       <c r="D8" s="18" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="F8" s="18" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="G8" s="18"/>
       <c r="H8" s="28"/>
@@ -1917,19 +1971,19 @@
         <v>7</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="H9" s="28"/>
     </row>
@@ -1942,16 +1996,16 @@
         <v>0</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E10" s="18" t="s">
         <v>6</v>
       </c>
       <c r="F10" s="18" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="G10" s="18" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H10" s="28"/>
     </row>
@@ -1961,22 +2015,22 @@
         <v>9</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E11" s="17" t="s">
         <v>11</v>
       </c>
       <c r="F11" s="18" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="G11" s="18" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -1985,19 +2039,19 @@
         <v>10</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F12" s="18" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="G12" s="29" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="H12" s="28"/>
     </row>
@@ -2007,16 +2061,16 @@
         <v>11</v>
       </c>
       <c r="C13" s="20" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E13" s="18" t="s">
         <v>9</v>
       </c>
       <c r="F13" s="18" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="G13" s="18"/>
       <c r="H13" s="28"/>
@@ -2027,20 +2081,20 @@
         <v>12</v>
       </c>
       <c r="C14" s="20" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F14" s="18" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="G14" s="18"/>
       <c r="H14" s="10" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="46.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -2049,20 +2103,20 @@
         <v>13</v>
       </c>
       <c r="C15" s="20" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F15" s="18" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="G15" s="18"/>
       <c r="H15" s="10" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -2074,16 +2128,16 @@
         <v>1</v>
       </c>
       <c r="D16" s="24" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E16" s="18" t="s">
         <v>5</v>
       </c>
       <c r="F16" s="18" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G16" s="18" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="H16" s="28"/>
     </row>
@@ -2093,19 +2147,19 @@
         <v>15</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D17" s="24" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E17" s="17" t="s">
         <v>8</v>
       </c>
       <c r="F17" s="30" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="G17" s="18" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="H17" s="28"/>
     </row>
@@ -2115,19 +2169,19 @@
         <v>16</v>
       </c>
       <c r="C18" s="20" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E18" s="17" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F18" s="18" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="G18" s="18" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H18" s="28"/>
     </row>
@@ -2137,14 +2191,14 @@
         <v>17</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D19" s="18"/>
       <c r="E19" s="17" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F19" s="30" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G19" s="18"/>
       <c r="H19" s="12"/>
@@ -2155,17 +2209,17 @@
         <v>18</v>
       </c>
       <c r="C20" s="20" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E20" s="23" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F20" s="18"/>
       <c r="G20" s="18" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H20" s="28"/>
     </row>
@@ -2175,17 +2229,17 @@
         <v>19</v>
       </c>
       <c r="C21" s="20" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E21" s="23" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F21" s="18"/>
       <c r="G21" s="18" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H21" s="28"/>
     </row>
@@ -2195,22 +2249,22 @@
         <v>20</v>
       </c>
       <c r="C22" s="20" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D22" s="23" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="E22" s="17" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F22" s="23" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G22" s="18" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="H22" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -2219,19 +2273,19 @@
         <v>21</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D23" s="23" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E23" s="23" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F23" s="23" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="G23" s="18" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="H23" s="28"/>
     </row>
@@ -2241,19 +2295,19 @@
         <v>22</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D24" s="23" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="E24" s="23" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F24" s="18" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="G24" s="18" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="H24" s="28"/>
     </row>
@@ -2263,19 +2317,19 @@
         <v>23</v>
       </c>
       <c r="C25" s="20" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D25" s="23" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E25" s="23" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F25" s="18" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="G25" s="18" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="H25" s="12"/>
     </row>
@@ -2285,19 +2339,19 @@
         <v>24</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D26" s="23" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E26" s="23" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F26" s="18" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="G26" s="18" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H26" s="12"/>
     </row>
@@ -2307,19 +2361,19 @@
         <v>25</v>
       </c>
       <c r="C27" s="20" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D27" s="23" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E27" s="23" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F27" s="18" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="G27" s="18" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="H27" s="12"/>
     </row>
@@ -2329,19 +2383,19 @@
         <v>26</v>
       </c>
       <c r="C28" s="20" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D28" s="23" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E28" s="23" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F28" s="18" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="G28" s="18" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="H28" s="12"/>
     </row>
@@ -2351,22 +2405,22 @@
         <v>27</v>
       </c>
       <c r="C29" s="20" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D29" s="23" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E29" s="23" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F29" s="18" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G29" s="18" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="H29" s="11" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2375,18 +2429,18 @@
         <v>28</v>
       </c>
       <c r="C30" s="23" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D30" s="23"/>
       <c r="E30" s="23" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F30" s="18" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G30" s="18"/>
       <c r="H30" s="11" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -2395,19 +2449,19 @@
         <v>29</v>
       </c>
       <c r="C31" s="20" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D31" s="23" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E31" s="23" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F31" s="18" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="G31" s="18" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="H31" s="28"/>
     </row>
@@ -2417,22 +2471,22 @@
         <v>31</v>
       </c>
       <c r="C32" s="20" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D32" s="23" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E32" s="23" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F32" s="27" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G32" s="18" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="H32" s="10" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="76.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -2441,22 +2495,22 @@
         <v>32</v>
       </c>
       <c r="C33" s="20" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D33" s="23" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E33" s="23" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F33" s="27" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G33" s="18" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="H33" s="10" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2465,19 +2519,19 @@
         <v>33</v>
       </c>
       <c r="C34" s="20" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D34" s="23" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E34" s="23" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F34" s="18" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="G34" s="18" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H34" s="28"/>
     </row>
@@ -2487,19 +2541,19 @@
         <v>34</v>
       </c>
       <c r="C35" s="30" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D35" s="23" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E35" s="23" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F35" s="30" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="G35" s="18" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="H35" s="28"/>
     </row>
@@ -2509,14 +2563,14 @@
         <v>35</v>
       </c>
       <c r="C36" s="23" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D36" s="23"/>
       <c r="E36" s="23" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F36" s="30" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G36" s="18"/>
       <c r="H36" s="12"/>
@@ -2527,19 +2581,19 @@
         <v>36</v>
       </c>
       <c r="C37" s="20" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D37" s="23" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E37" s="23" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F37" s="18" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="G37" s="27" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="H37" s="28"/>
     </row>
@@ -2549,19 +2603,19 @@
         <v>37</v>
       </c>
       <c r="C38" s="20" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D38" s="23" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E38" s="23" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F38" s="18" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="G38" s="27" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="H38" s="28"/>
     </row>
@@ -2571,14 +2625,14 @@
         <v>38</v>
       </c>
       <c r="C39" s="23" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D39" s="23"/>
       <c r="E39" s="23" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F39" s="30" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G39" s="18"/>
       <c r="H39" s="12"/>
@@ -2589,19 +2643,19 @@
         <v>39</v>
       </c>
       <c r="C40" s="20" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D40" s="23" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E40" s="23" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F40" s="18" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="G40" s="18" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="H40" s="12"/>
     </row>
@@ -2611,19 +2665,19 @@
         <v>40</v>
       </c>
       <c r="C41" s="20" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D41" s="23" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E41" s="23" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F41" s="19" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="G41" s="18" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="H41" s="12"/>
     </row>
@@ -2633,18 +2687,18 @@
         <v>41</v>
       </c>
       <c r="C42" s="21" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D42" s="23"/>
       <c r="E42" s="23" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F42" s="30" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G42" s="18"/>
       <c r="H42" s="11" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -2653,16 +2707,16 @@
         <v>45</v>
       </c>
       <c r="C43" s="20" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D43" s="23" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E43" s="23" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="F43" s="18" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="G43" s="18"/>
       <c r="H43" s="28"/>
@@ -2673,16 +2727,16 @@
         <v>46</v>
       </c>
       <c r="C44" s="20" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D44" s="23" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E44" s="23" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="F44" s="18" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="G44" s="18"/>
       <c r="H44" s="28"/>
@@ -2693,19 +2747,19 @@
         <v>47</v>
       </c>
       <c r="C45" s="20" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D45" s="23" t="s">
+        <v>189</v>
+      </c>
+      <c r="E45" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="F45" s="18" t="s">
+        <v>226</v>
+      </c>
+      <c r="G45" s="27" t="s">
         <v>191</v>
-      </c>
-      <c r="E45" s="23" t="s">
-        <v>109</v>
-      </c>
-      <c r="F45" s="18" t="s">
-        <v>228</v>
-      </c>
-      <c r="G45" s="27" t="s">
-        <v>193</v>
       </c>
       <c r="H45" s="28"/>
     </row>
@@ -2715,19 +2769,19 @@
         <v>48</v>
       </c>
       <c r="C46" s="20" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D46" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="E46" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="F46" s="18" t="s">
+        <v>226</v>
+      </c>
+      <c r="G46" s="27" t="s">
         <v>192</v>
-      </c>
-      <c r="E46" s="23" t="s">
-        <v>110</v>
-      </c>
-      <c r="F46" s="18" t="s">
-        <v>228</v>
-      </c>
-      <c r="G46" s="27" t="s">
-        <v>194</v>
       </c>
       <c r="H46" s="28"/>
     </row>
@@ -2737,14 +2791,14 @@
         <v>49</v>
       </c>
       <c r="C47" s="19" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D47" s="24"/>
       <c r="E47" s="23" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F47" s="18" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="G47" s="27"/>
       <c r="H47" s="28"/>
@@ -2755,14 +2809,14 @@
         <v>50</v>
       </c>
       <c r="C48" s="19" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D48" s="24"/>
       <c r="E48" s="23" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="F48" s="18" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="G48" s="27"/>
       <c r="H48" s="28"/>
@@ -2773,14 +2827,14 @@
         <v>51</v>
       </c>
       <c r="C49" s="19" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D49" s="24"/>
       <c r="E49" s="23" t="s">
+        <v>252</v>
+      </c>
+      <c r="F49" s="18" t="s">
         <v>254</v>
-      </c>
-      <c r="F49" s="18" t="s">
-        <v>256</v>
       </c>
       <c r="G49" s="27"/>
       <c r="H49" s="28"/>
@@ -2791,14 +2845,14 @@
         <v>52</v>
       </c>
       <c r="C50" s="19" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D50" s="24"/>
       <c r="E50" s="23" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="F50" s="18" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="G50" s="27"/>
       <c r="H50" s="28"/>
@@ -2810,36 +2864,36 @@
       </c>
       <c r="C51" s="24"/>
       <c r="D51" s="24" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E51" s="23"/>
       <c r="F51" s="18"/>
       <c r="G51" s="27" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="H51" s="28"/>
     </row>
     <row r="52" spans="1:8" ht="57.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="32" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B52" s="26">
         <v>1</v>
       </c>
       <c r="C52" s="24" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D52" s="24" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E52" s="24" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F52" s="18" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="G52" s="18" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="H52" s="28"/>
     </row>
@@ -2849,19 +2903,19 @@
         <v>2</v>
       </c>
       <c r="C53" s="24" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D53" s="24" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E53" s="24" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F53" s="18" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="G53" s="18" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="H53" s="28"/>
     </row>
@@ -2881,10 +2935,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C47"/>
+  <dimension ref="A1:C49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2902,10 +2956,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" s="40" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>263</v>
+        <v>261</v>
+      </c>
+      <c r="C1" s="43" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
@@ -2913,13 +2970,14 @@
       <c r="B2" s="6" t="s">
         <v>17</v>
       </c>
+      <c r="C2" s="43"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" s="40" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
@@ -2936,7 +2994,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A6" s="40" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>28</v>
@@ -2950,10 +3008,13 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A8" s="40" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>54</v>
+      </c>
+      <c r="C8" s="43" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
@@ -2961,10 +3022,11 @@
       <c r="B9" s="6" t="s">
         <v>55</v>
       </c>
+      <c r="C9" s="43"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A10" s="31" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>56</v>
@@ -2972,10 +3034,13 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A11" s="39" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>57</v>
+      </c>
+      <c r="C11" s="43" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.15">
@@ -2983,271 +3048,300 @@
       <c r="B12" s="6" t="s">
         <v>58</v>
       </c>
+      <c r="C12" s="43"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A13" s="39" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>59</v>
+        <v>265</v>
+      </c>
+      <c r="C13" s="43" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A14" s="39"/>
       <c r="B14" s="6" t="s">
-        <v>60</v>
-      </c>
+        <v>262</v>
+      </c>
+      <c r="C14" s="43"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A15" s="39" t="s">
-        <v>61</v>
-      </c>
-      <c r="B15" s="5" t="s">
+      <c r="A15" s="41" t="s">
+        <v>264</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="C15" s="43" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A16" s="42"/>
+      <c r="B16" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="C16" s="44"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A17" s="39" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="36" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A16" s="39"/>
-      <c r="B16" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" s="37"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A17" s="39"/>
-      <c r="B17" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17" s="37"/>
+      <c r="C17" s="36" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A18" s="39"/>
       <c r="B18" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C18" s="37"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A19" s="39"/>
       <c r="B19" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C19" s="37"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A20" s="39"/>
       <c r="B20" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C20" s="37"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A21" s="39"/>
       <c r="B21" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C21" s="37"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A22" s="39"/>
       <c r="B22" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C22" s="37"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A23" s="39" t="s">
-        <v>63</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>31</v>
+      <c r="A23" s="39"/>
+      <c r="B23" s="5" t="s">
+        <v>26</v>
       </c>
       <c r="C23" s="37"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A24" s="39"/>
-      <c r="B24" s="6" t="s">
-        <v>34</v>
+      <c r="B24" s="5" t="s">
+        <v>27</v>
       </c>
       <c r="C24" s="37"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A25" s="39"/>
+      <c r="A25" s="39" t="s">
+        <v>61</v>
+      </c>
       <c r="B25" s="6" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C25" s="37"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A26" s="39"/>
       <c r="B26" s="6" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C26" s="37"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A27" s="39"/>
       <c r="B27" s="6" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C27" s="37"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A28" s="39"/>
       <c r="B28" s="6" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C28" s="37"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A29" s="39"/>
       <c r="B29" s="6" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C29" s="37"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A30" s="39"/>
       <c r="B30" s="6" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C30" s="37"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A31" s="39" t="s">
-        <v>64</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>30</v>
+      <c r="A31" s="39"/>
+      <c r="B31" s="6" t="s">
+        <v>49</v>
       </c>
       <c r="C31" s="37"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A32" s="39"/>
-      <c r="B32" s="7" t="s">
-        <v>33</v>
+      <c r="B32" s="6" t="s">
+        <v>52</v>
       </c>
       <c r="C32" s="37"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A33" s="39"/>
+      <c r="A33" s="39" t="s">
+        <v>62</v>
+      </c>
       <c r="B33" s="7" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C33" s="37"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A34" s="39"/>
       <c r="B34" s="7" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C34" s="37"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A35" s="39"/>
       <c r="B35" s="7" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C35" s="37"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A36" s="39"/>
       <c r="B36" s="7" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C36" s="37"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A37" s="39"/>
       <c r="B37" s="7" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C37" s="37"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A38" s="39"/>
       <c r="B38" s="7" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C38" s="37"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A39" s="39" t="s">
-        <v>65</v>
-      </c>
-      <c r="B39" s="8" t="s">
-        <v>29</v>
+      <c r="A39" s="39"/>
+      <c r="B39" s="7" t="s">
+        <v>48</v>
       </c>
       <c r="C39" s="37"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A40" s="39"/>
-      <c r="B40" s="8" t="s">
-        <v>32</v>
+      <c r="B40" s="7" t="s">
+        <v>51</v>
       </c>
       <c r="C40" s="37"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A41" s="39"/>
+      <c r="A41" s="39" t="s">
+        <v>63</v>
+      </c>
       <c r="B41" s="8" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C41" s="37"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A42" s="39"/>
       <c r="B42" s="8" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C42" s="37"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A43" s="39"/>
       <c r="B43" s="8" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C43" s="37"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A44" s="39"/>
       <c r="B44" s="8" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C44" s="37"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A45" s="39"/>
       <c r="B45" s="8" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C45" s="37"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A46" s="39"/>
       <c r="B46" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C46" s="37"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A47" s="39"/>
+      <c r="B47" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C47" s="37"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A48" s="39"/>
+      <c r="B48" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="C46" s="38"/>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A47" s="9"/>
+      <c r="C48" s="38"/>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A49" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="C15:C46"/>
-    <mergeCell ref="A15:A22"/>
+  <mergeCells count="17">
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="C17:C48"/>
+    <mergeCell ref="A17:A24"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A23:A30"/>
-    <mergeCell ref="A31:A38"/>
-    <mergeCell ref="A39:A46"/>
+    <mergeCell ref="A25:A32"/>
+    <mergeCell ref="A33:A40"/>
+    <mergeCell ref="A41:A48"/>
     <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="C8:C9"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add comments in Set_Led command
</commit_message>
<xml_diff>
--- a/R1_test_command_list_tag1.7PTE.xlsx
+++ b/R1_test_command_list_tag1.7PTE.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="commands_list" sheetId="1" r:id="rId1"/>
@@ -48,9 +48,6 @@
     <t>Set Wlan0 Mac address</t>
   </si>
   <si>
-    <t>Set leds</t>
-  </si>
-  <si>
     <t>Check buttons</t>
   </si>
   <si>
@@ -72,139 +69,58 @@
     <t>#</t>
   </si>
   <si>
-    <t>ACTION_r</t>
-  </si>
-  <si>
-    <t>CONNECT_g</t>
-  </si>
-  <si>
-    <t>CONNECT_r</t>
-  </si>
-  <si>
-    <t>Lantern_W1_g</t>
-  </si>
-  <si>
-    <t>Lantern_W1_r</t>
-  </si>
-  <si>
-    <t>Lantern_W2_b</t>
-  </si>
-  <si>
-    <t>Lantern_W2_g</t>
-  </si>
-  <si>
-    <t>Lantern_W2_r</t>
-  </si>
-  <si>
-    <t>Lantern_W3_b</t>
-  </si>
-  <si>
-    <t>Lantern_W3_g</t>
-  </si>
-  <si>
     <t>Lantern_W3_r</t>
   </si>
   <si>
-    <t>Lantern_g</t>
-  </si>
-  <si>
     <t>Lantern_led1_b</t>
   </si>
   <si>
-    <t>Lantern_led1_g</t>
-  </si>
-  <si>
-    <t>Lantern_led1_r</t>
-  </si>
-  <si>
     <t>Lantern_led2_b</t>
   </si>
   <si>
     <t>Lantern_led2_g</t>
   </si>
   <si>
-    <t>Lantern_led2_r</t>
-  </si>
-  <si>
     <t>Lantern_led3_b</t>
   </si>
   <si>
     <t>Lantern_led3_g</t>
   </si>
   <si>
-    <t>Lantern_led3_r</t>
-  </si>
-  <si>
     <t>Lantern_led4_b</t>
   </si>
   <si>
     <t>Lantern_led4_g</t>
   </si>
   <si>
-    <t>Lantern_led4_r</t>
-  </si>
-  <si>
     <t>Lantern_led5_b</t>
   </si>
   <si>
     <t>Lantern_led5_g</t>
   </si>
   <si>
-    <t>Lantern_led5_r</t>
-  </si>
-  <si>
     <t>Lantern_led6_b</t>
   </si>
   <si>
     <t>Lantern_led6_g</t>
   </si>
   <si>
-    <t>Lantern_led6_r</t>
-  </si>
-  <si>
     <t>Lantern_led7_b</t>
   </si>
   <si>
     <t>Lantern_led7_g</t>
   </si>
   <si>
-    <t>Lantern_led7_r</t>
-  </si>
-  <si>
     <t>Lantern_led8_b</t>
   </si>
   <si>
     <t>Lantern_led8_g</t>
   </si>
   <si>
-    <t>Lantern_led8_r</t>
-  </si>
-  <si>
-    <t>Lantern_r</t>
-  </si>
-  <si>
-    <t>PLAYPAUSE_g</t>
-  </si>
-  <si>
-    <t>PLAYPAUSE_r</t>
-  </si>
-  <si>
-    <t>USB_r</t>
-  </si>
-  <si>
-    <t>VOL+_g</t>
-  </si>
-  <si>
-    <t>VOL+_r</t>
-  </si>
-  <si>
     <t>Lantern White</t>
   </si>
   <si>
     <t>Connect Key</t>
-  </si>
-  <si>
-    <t>Lantern Red</t>
   </si>
   <si>
     <t>Lantern Green</t>
@@ -260,10 +176,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>CONNECT_b</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>adb shell /etc/factory-test/r1/set_shutdown.sh</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -715,10 +627,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>adb shell /etc/factory-test/r1/set_led.sh ACTION_r 113</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>./set_led.sh &lt;led_name&gt; &lt;0..255&gt;</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -855,10 +763,6 @@
   </si>
   <si>
     <t>./set_lantern_on.sh</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>./set_lantern_off.sh</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1094,43 +998,167 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>Mute Key</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mute_g</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Only White/Red for Mute key</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Volume- Key</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Only White for Volume- key</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Only White for Pause key</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Only White for Action key</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Only White for Volume+ key</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lantern_W1_g</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lantern_W1_r</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>./set_lantern_off.sh</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lantern_W2_b</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lantern_W2_g</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lantern_W2_r</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lantern_W3_b</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lantern_W3_g</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lantern Red</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lantern_led1_r</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lantern_led2_r</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lantern_led3_r</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lantern_led4_r</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lantern_led5_r</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lantern_led6_r</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lantern_led7_r</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lantern_led8_r</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lantern_led1_g</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ACTION_r</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CONNECT_g</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CONNECT_r</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VOL-_g</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CONNECT_b</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lantern_g</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lantern_r</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PLAYPAUSE_g</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PLAYPAUSE_r</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>USB_r</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VOL+_g</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VOL+_r</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Mute_r</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Mute Key</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>VOL-_g</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Mute_g</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Only White/Red for Mute key</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Volume- Key</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Only White for Volume- key</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Only White for Pause key</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Only White for Action key</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Only White for Volume+ key</t>
+    <t>adb shell /etc/factory-test/r1/set_led.sh ACTION_r 113</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Set leds， the led name (for example: ACTION_r) must match with the leds_names list</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1786,8 +1814,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H58"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1805,52 +1833,52 @@
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="15" t="s">
-        <v>85</v>
+        <v>56</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C1" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="E1" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="16" t="s">
-        <v>15</v>
-      </c>
       <c r="F1" s="16" t="s">
-        <v>86</v>
+        <v>57</v>
       </c>
       <c r="G1" s="16" t="s">
-        <v>79</v>
+        <v>50</v>
       </c>
       <c r="H1" s="16" t="s">
-        <v>82</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="41.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="33" t="s">
-        <v>84</v>
+        <v>55</v>
       </c>
       <c r="B2" s="25">
         <v>1</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>111</v>
+        <v>82</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>68</v>
+        <v>40</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>225</v>
+        <v>194</v>
       </c>
       <c r="G2" s="18"/>
       <c r="H2" s="10" t="s">
-        <v>167</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="99.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1859,19 +1887,19 @@
         <v>2</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>160</v>
+        <v>131</v>
       </c>
       <c r="D3" s="24" t="s">
-        <v>116</v>
+        <v>87</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>248</v>
+        <v>217</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>225</v>
+        <v>194</v>
       </c>
       <c r="G3" s="18" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="H3" s="28"/>
     </row>
@@ -1884,16 +1912,16 @@
         <v>2</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>66</v>
+        <v>38</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>80</v>
+        <v>51</v>
       </c>
       <c r="F4" s="18" t="s">
-        <v>225</v>
+        <v>194</v>
       </c>
       <c r="G4" s="18" t="s">
-        <v>121</v>
+        <v>92</v>
       </c>
       <c r="H4" s="28"/>
     </row>
@@ -1906,16 +1934,16 @@
         <v>3</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>67</v>
+        <v>39</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>81</v>
+        <v>52</v>
       </c>
       <c r="F5" s="18" t="s">
-        <v>225</v>
+        <v>194</v>
       </c>
       <c r="G5" s="18" t="s">
-        <v>122</v>
+        <v>93</v>
       </c>
       <c r="H5" s="28"/>
     </row>
@@ -1925,19 +1953,19 @@
         <v>5</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>118</v>
+        <v>89</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>114</v>
+        <v>85</v>
       </c>
       <c r="E6" s="18" t="s">
         <v>7</v>
       </c>
       <c r="F6" s="18" t="s">
-        <v>225</v>
+        <v>194</v>
       </c>
       <c r="G6" s="18" t="s">
-        <v>119</v>
+        <v>90</v>
       </c>
       <c r="H6" s="28"/>
     </row>
@@ -1950,13 +1978,13 @@
         <v>4</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>65</v>
+        <v>37</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F7" s="18" t="s">
-        <v>225</v>
+        <v>194</v>
       </c>
       <c r="G7" s="18"/>
       <c r="H7" s="28"/>
@@ -1966,13 +1994,13 @@
       <c r="B8" s="25"/>
       <c r="C8" s="20"/>
       <c r="D8" s="18" t="s">
-        <v>239</v>
+        <v>208</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>228</v>
+        <v>197</v>
       </c>
       <c r="F8" s="18" t="s">
-        <v>229</v>
+        <v>198</v>
       </c>
       <c r="G8" s="18"/>
       <c r="H8" s="28"/>
@@ -1983,19 +2011,19 @@
         <v>7</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>120</v>
+        <v>91</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>115</v>
+        <v>86</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>87</v>
+        <v>58</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>230</v>
+        <v>199</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>227</v>
+        <v>196</v>
       </c>
       <c r="H9" s="28"/>
     </row>
@@ -2008,16 +2036,16 @@
         <v>0</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>69</v>
+        <v>41</v>
       </c>
       <c r="E10" s="18" t="s">
         <v>6</v>
       </c>
       <c r="F10" s="18" t="s">
-        <v>226</v>
+        <v>195</v>
       </c>
       <c r="G10" s="18" t="s">
-        <v>176</v>
+        <v>147</v>
       </c>
       <c r="H10" s="28"/>
     </row>
@@ -2027,22 +2055,22 @@
         <v>9</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>123</v>
+        <v>94</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>112</v>
+        <v>83</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F11" s="18" t="s">
-        <v>226</v>
+        <v>195</v>
       </c>
       <c r="G11" s="18" t="s">
-        <v>177</v>
+        <v>148</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>208</v>
+        <v>178</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -2051,19 +2079,19 @@
         <v>10</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>124</v>
+        <v>95</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>113</v>
+        <v>84</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>179</v>
+        <v>150</v>
       </c>
       <c r="F12" s="18" t="s">
-        <v>226</v>
+        <v>195</v>
       </c>
       <c r="G12" s="29" t="s">
-        <v>178</v>
+        <v>149</v>
       </c>
       <c r="H12" s="28"/>
     </row>
@@ -2073,16 +2101,16 @@
         <v>11</v>
       </c>
       <c r="C13" s="20" t="s">
-        <v>181</v>
+        <v>151</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>180</v>
+        <v>270</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>9</v>
+        <v>271</v>
       </c>
       <c r="F13" s="18" t="s">
-        <v>226</v>
+        <v>195</v>
       </c>
       <c r="G13" s="18"/>
       <c r="H13" s="28"/>
@@ -2093,20 +2121,20 @@
         <v>12</v>
       </c>
       <c r="C14" s="20" t="s">
-        <v>215</v>
+        <v>185</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>182</v>
+        <v>152</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>169</v>
+        <v>140</v>
       </c>
       <c r="F14" s="18" t="s">
-        <v>226</v>
+        <v>195</v>
       </c>
       <c r="G14" s="18"/>
       <c r="H14" s="10" t="s">
-        <v>203</v>
+        <v>173</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="46.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -2115,20 +2143,20 @@
         <v>13</v>
       </c>
       <c r="C15" s="20" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>217</v>
+        <v>186</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>170</v>
+        <v>141</v>
       </c>
       <c r="F15" s="18" t="s">
-        <v>226</v>
+        <v>195</v>
       </c>
       <c r="G15" s="18"/>
       <c r="H15" s="10" t="s">
-        <v>203</v>
+        <v>173</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -2140,16 +2168,16 @@
         <v>1</v>
       </c>
       <c r="D16" s="24" t="s">
-        <v>71</v>
+        <v>42</v>
       </c>
       <c r="E16" s="18" t="s">
         <v>5</v>
       </c>
       <c r="F16" s="18" t="s">
-        <v>225</v>
+        <v>194</v>
       </c>
       <c r="G16" s="18" t="s">
-        <v>125</v>
+        <v>96</v>
       </c>
       <c r="H16" s="28"/>
     </row>
@@ -2159,19 +2187,19 @@
         <v>15</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>128</v>
+        <v>99</v>
       </c>
       <c r="D17" s="24" t="s">
-        <v>117</v>
+        <v>88</v>
       </c>
       <c r="E17" s="17" t="s">
         <v>8</v>
       </c>
       <c r="F17" s="30" t="s">
-        <v>246</v>
+        <v>215</v>
       </c>
       <c r="G17" s="18" t="s">
-        <v>245</v>
+        <v>214</v>
       </c>
       <c r="H17" s="28"/>
     </row>
@@ -2181,19 +2209,19 @@
         <v>16</v>
       </c>
       <c r="C18" s="20" t="s">
-        <v>129</v>
+        <v>100</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>126</v>
+        <v>97</v>
       </c>
       <c r="E18" s="17" t="s">
-        <v>99</v>
+        <v>70</v>
       </c>
       <c r="F18" s="18" t="s">
-        <v>226</v>
+        <v>195</v>
       </c>
       <c r="G18" s="18" t="s">
-        <v>127</v>
+        <v>98</v>
       </c>
       <c r="H18" s="28"/>
     </row>
@@ -2203,14 +2231,14 @@
         <v>17</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>72</v>
+        <v>43</v>
       </c>
       <c r="D19" s="18"/>
       <c r="E19" s="17" t="s">
-        <v>88</v>
+        <v>59</v>
       </c>
       <c r="F19" s="30" t="s">
-        <v>159</v>
+        <v>130</v>
       </c>
       <c r="G19" s="18"/>
       <c r="H19" s="12"/>
@@ -2221,17 +2249,17 @@
         <v>18</v>
       </c>
       <c r="C20" s="20" t="s">
-        <v>133</v>
+        <v>104</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>130</v>
+        <v>101</v>
       </c>
       <c r="E20" s="23" t="s">
-        <v>89</v>
+        <v>60</v>
       </c>
       <c r="F20" s="18"/>
       <c r="G20" s="18" t="s">
-        <v>131</v>
+        <v>102</v>
       </c>
       <c r="H20" s="28"/>
     </row>
@@ -2241,17 +2269,17 @@
         <v>19</v>
       </c>
       <c r="C21" s="20" t="s">
-        <v>134</v>
+        <v>105</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>183</v>
+        <v>153</v>
       </c>
       <c r="E21" s="23" t="s">
-        <v>89</v>
+        <v>60</v>
       </c>
       <c r="F21" s="18"/>
       <c r="G21" s="18" t="s">
-        <v>132</v>
+        <v>103</v>
       </c>
       <c r="H21" s="28"/>
     </row>
@@ -2261,22 +2289,22 @@
         <v>20</v>
       </c>
       <c r="C22" s="20" t="s">
-        <v>184</v>
+        <v>154</v>
       </c>
       <c r="D22" s="23" t="s">
-        <v>237</v>
+        <v>206</v>
       </c>
       <c r="E22" s="17" t="s">
-        <v>100</v>
+        <v>71</v>
       </c>
       <c r="F22" s="23" t="s">
-        <v>225</v>
+        <v>194</v>
       </c>
       <c r="G22" s="18" t="s">
-        <v>238</v>
+        <v>207</v>
       </c>
       <c r="H22" s="10" t="s">
-        <v>209</v>
+        <v>179</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -2285,19 +2313,19 @@
         <v>21</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>135</v>
+        <v>106</v>
       </c>
       <c r="D23" s="23" t="s">
-        <v>233</v>
+        <v>202</v>
       </c>
       <c r="E23" s="23" t="s">
-        <v>101</v>
+        <v>72</v>
       </c>
       <c r="F23" s="23" t="s">
-        <v>229</v>
+        <v>198</v>
       </c>
       <c r="G23" s="18" t="s">
-        <v>236</v>
+        <v>205</v>
       </c>
       <c r="H23" s="28"/>
     </row>
@@ -2307,19 +2335,19 @@
         <v>22</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>136</v>
+        <v>107</v>
       </c>
       <c r="D24" s="23" t="s">
-        <v>234</v>
+        <v>203</v>
       </c>
       <c r="E24" s="23" t="s">
-        <v>90</v>
+        <v>61</v>
       </c>
       <c r="F24" s="18" t="s">
-        <v>229</v>
+        <v>198</v>
       </c>
       <c r="G24" s="18" t="s">
-        <v>235</v>
+        <v>204</v>
       </c>
       <c r="H24" s="28"/>
     </row>
@@ -2329,19 +2357,19 @@
         <v>23</v>
       </c>
       <c r="C25" s="20" t="s">
-        <v>139</v>
+        <v>110</v>
       </c>
       <c r="D25" s="23" t="s">
-        <v>137</v>
+        <v>108</v>
       </c>
       <c r="E25" s="23" t="s">
-        <v>91</v>
+        <v>62</v>
       </c>
       <c r="F25" s="18" t="s">
-        <v>226</v>
+        <v>195</v>
       </c>
       <c r="G25" s="18" t="s">
-        <v>138</v>
+        <v>109</v>
       </c>
       <c r="H25" s="12"/>
     </row>
@@ -2351,19 +2379,19 @@
         <v>24</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>142</v>
+        <v>113</v>
       </c>
       <c r="D26" s="23" t="s">
-        <v>140</v>
+        <v>111</v>
       </c>
       <c r="E26" s="23" t="s">
-        <v>92</v>
+        <v>63</v>
       </c>
       <c r="F26" s="18" t="s">
-        <v>226</v>
+        <v>195</v>
       </c>
       <c r="G26" s="18" t="s">
-        <v>141</v>
+        <v>112</v>
       </c>
       <c r="H26" s="12"/>
     </row>
@@ -2373,19 +2401,19 @@
         <v>25</v>
       </c>
       <c r="C27" s="20" t="s">
-        <v>145</v>
+        <v>116</v>
       </c>
       <c r="D27" s="23" t="s">
-        <v>143</v>
+        <v>114</v>
       </c>
       <c r="E27" s="23" t="s">
-        <v>93</v>
+        <v>64</v>
       </c>
       <c r="F27" s="18" t="s">
-        <v>226</v>
+        <v>195</v>
       </c>
       <c r="G27" s="18" t="s">
-        <v>144</v>
+        <v>115</v>
       </c>
       <c r="H27" s="12"/>
     </row>
@@ -2395,19 +2423,19 @@
         <v>26</v>
       </c>
       <c r="C28" s="20" t="s">
-        <v>148</v>
+        <v>119</v>
       </c>
       <c r="D28" s="23" t="s">
-        <v>146</v>
+        <v>117</v>
       </c>
       <c r="E28" s="23" t="s">
-        <v>94</v>
+        <v>65</v>
       </c>
       <c r="F28" s="18" t="s">
-        <v>226</v>
+        <v>195</v>
       </c>
       <c r="G28" s="18" t="s">
-        <v>147</v>
+        <v>118</v>
       </c>
       <c r="H28" s="12"/>
     </row>
@@ -2417,22 +2445,22 @@
         <v>27</v>
       </c>
       <c r="C29" s="20" t="s">
-        <v>185</v>
+        <v>155</v>
       </c>
       <c r="D29" s="23" t="s">
-        <v>149</v>
+        <v>120</v>
       </c>
       <c r="E29" s="23" t="s">
-        <v>166</v>
+        <v>137</v>
       </c>
       <c r="F29" s="18" t="s">
-        <v>225</v>
+        <v>194</v>
       </c>
       <c r="G29" s="18" t="s">
-        <v>202</v>
+        <v>172</v>
       </c>
       <c r="H29" s="11" t="s">
-        <v>173</v>
+        <v>144</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2441,18 +2469,18 @@
         <v>28</v>
       </c>
       <c r="C30" s="23" t="s">
-        <v>73</v>
+        <v>44</v>
       </c>
       <c r="D30" s="23"/>
       <c r="E30" s="23" t="s">
-        <v>102</v>
+        <v>73</v>
       </c>
       <c r="F30" s="18" t="s">
-        <v>168</v>
+        <v>139</v>
       </c>
       <c r="G30" s="18"/>
       <c r="H30" s="11" t="s">
-        <v>174</v>
+        <v>145</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -2461,19 +2489,19 @@
         <v>29</v>
       </c>
       <c r="C31" s="20" t="s">
-        <v>151</v>
+        <v>122</v>
       </c>
       <c r="D31" s="23" t="s">
-        <v>218</v>
+        <v>187</v>
       </c>
       <c r="E31" s="23" t="s">
-        <v>95</v>
+        <v>66</v>
       </c>
       <c r="F31" s="18" t="s">
-        <v>229</v>
+        <v>198</v>
       </c>
       <c r="G31" s="18" t="s">
-        <v>150</v>
+        <v>121</v>
       </c>
       <c r="H31" s="28"/>
     </row>
@@ -2483,22 +2511,22 @@
         <v>31</v>
       </c>
       <c r="C32" s="20" t="s">
-        <v>200</v>
+        <v>170</v>
       </c>
       <c r="D32" s="23" t="s">
-        <v>198</v>
+        <v>168</v>
       </c>
       <c r="E32" s="23" t="s">
-        <v>171</v>
+        <v>142</v>
       </c>
       <c r="F32" s="27" t="s">
-        <v>225</v>
+        <v>194</v>
       </c>
       <c r="G32" s="18" t="s">
-        <v>199</v>
+        <v>169</v>
       </c>
       <c r="H32" s="10" t="s">
-        <v>210</v>
+        <v>180</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="76.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -2507,22 +2535,22 @@
         <v>32</v>
       </c>
       <c r="C33" s="20" t="s">
-        <v>201</v>
+        <v>171</v>
       </c>
       <c r="D33" s="23" t="s">
-        <v>186</v>
+        <v>156</v>
       </c>
       <c r="E33" s="23" t="s">
-        <v>172</v>
+        <v>143</v>
       </c>
       <c r="F33" s="27" t="s">
-        <v>225</v>
+        <v>194</v>
       </c>
       <c r="G33" s="18" t="s">
-        <v>197</v>
+        <v>167</v>
       </c>
       <c r="H33" s="10" t="s">
-        <v>210</v>
+        <v>180</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2531,19 +2559,19 @@
         <v>33</v>
       </c>
       <c r="C34" s="20" t="s">
-        <v>154</v>
+        <v>125</v>
       </c>
       <c r="D34" s="23" t="s">
-        <v>152</v>
+        <v>123</v>
       </c>
       <c r="E34" s="23" t="s">
-        <v>96</v>
+        <v>67</v>
       </c>
       <c r="F34" s="18" t="s">
-        <v>229</v>
+        <v>198</v>
       </c>
       <c r="G34" s="18" t="s">
-        <v>153</v>
+        <v>124</v>
       </c>
       <c r="H34" s="28"/>
     </row>
@@ -2553,19 +2581,19 @@
         <v>34</v>
       </c>
       <c r="C35" s="30" t="s">
-        <v>165</v>
+        <v>136</v>
       </c>
       <c r="D35" s="23" t="s">
-        <v>155</v>
+        <v>126</v>
       </c>
       <c r="E35" s="23" t="s">
-        <v>74</v>
+        <v>45</v>
       </c>
       <c r="F35" s="30" t="s">
-        <v>243</v>
+        <v>212</v>
       </c>
       <c r="G35" s="18" t="s">
-        <v>242</v>
+        <v>211</v>
       </c>
       <c r="H35" s="28"/>
     </row>
@@ -2575,14 +2603,14 @@
         <v>35</v>
       </c>
       <c r="C36" s="23" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="D36" s="23"/>
       <c r="E36" s="23" t="s">
-        <v>103</v>
+        <v>74</v>
       </c>
       <c r="F36" s="30" t="s">
-        <v>159</v>
+        <v>130</v>
       </c>
       <c r="G36" s="18"/>
       <c r="H36" s="12"/>
@@ -2593,19 +2621,19 @@
         <v>36</v>
       </c>
       <c r="C37" s="20" t="s">
-        <v>188</v>
+        <v>158</v>
       </c>
       <c r="D37" s="23" t="s">
-        <v>156</v>
+        <v>127</v>
       </c>
       <c r="E37" s="23" t="s">
-        <v>104</v>
+        <v>75</v>
       </c>
       <c r="F37" s="18" t="s">
-        <v>226</v>
+        <v>195</v>
       </c>
       <c r="G37" s="27" t="s">
-        <v>187</v>
+        <v>157</v>
       </c>
       <c r="H37" s="28"/>
     </row>
@@ -2615,19 +2643,19 @@
         <v>37</v>
       </c>
       <c r="C38" s="20" t="s">
-        <v>158</v>
+        <v>129</v>
       </c>
       <c r="D38" s="23" t="s">
-        <v>196</v>
+        <v>166</v>
       </c>
       <c r="E38" s="23" t="s">
-        <v>97</v>
+        <v>68</v>
       </c>
       <c r="F38" s="18" t="s">
-        <v>226</v>
+        <v>195</v>
       </c>
       <c r="G38" s="27" t="s">
-        <v>157</v>
+        <v>128</v>
       </c>
       <c r="H38" s="28"/>
     </row>
@@ -2637,14 +2665,14 @@
         <v>38</v>
       </c>
       <c r="C39" s="23" t="s">
-        <v>76</v>
+        <v>47</v>
       </c>
       <c r="D39" s="23"/>
       <c r="E39" s="23" t="s">
-        <v>105</v>
+        <v>76</v>
       </c>
       <c r="F39" s="30" t="s">
-        <v>159</v>
+        <v>130</v>
       </c>
       <c r="G39" s="18"/>
       <c r="H39" s="12"/>
@@ -2655,19 +2683,19 @@
         <v>39</v>
       </c>
       <c r="C40" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="D40" s="23" t="s">
+        <v>192</v>
+      </c>
+      <c r="E40" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="D40" s="23" t="s">
-        <v>223</v>
-      </c>
-      <c r="E40" s="23" t="s">
-        <v>106</v>
-      </c>
       <c r="F40" s="18" t="s">
-        <v>229</v>
+        <v>198</v>
       </c>
       <c r="G40" s="18" t="s">
-        <v>224</v>
+        <v>193</v>
       </c>
       <c r="H40" s="12"/>
     </row>
@@ -2677,19 +2705,19 @@
         <v>40</v>
       </c>
       <c r="C41" s="20" t="s">
-        <v>231</v>
+        <v>200</v>
       </c>
       <c r="D41" s="23" t="s">
-        <v>195</v>
+        <v>165</v>
       </c>
       <c r="E41" s="23" t="s">
-        <v>164</v>
+        <v>135</v>
       </c>
       <c r="F41" s="19" t="s">
-        <v>232</v>
+        <v>201</v>
       </c>
       <c r="G41" s="18" t="s">
-        <v>219</v>
+        <v>188</v>
       </c>
       <c r="H41" s="12"/>
     </row>
@@ -2699,18 +2727,18 @@
         <v>41</v>
       </c>
       <c r="C42" s="21" t="s">
-        <v>78</v>
+        <v>49</v>
       </c>
       <c r="D42" s="23"/>
       <c r="E42" s="23" t="s">
-        <v>98</v>
+        <v>69</v>
       </c>
       <c r="F42" s="30" t="s">
-        <v>159</v>
+        <v>130</v>
       </c>
       <c r="G42" s="18"/>
       <c r="H42" s="11" t="s">
-        <v>175</v>
+        <v>146</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -2719,16 +2747,16 @@
         <v>45</v>
       </c>
       <c r="C43" s="20" t="s">
-        <v>240</v>
+        <v>209</v>
       </c>
       <c r="D43" s="23" t="s">
-        <v>211</v>
+        <v>181</v>
       </c>
       <c r="E43" s="23" t="s">
-        <v>204</v>
+        <v>174</v>
       </c>
       <c r="F43" s="18" t="s">
-        <v>229</v>
+        <v>198</v>
       </c>
       <c r="G43" s="18"/>
       <c r="H43" s="28"/>
@@ -2739,16 +2767,16 @@
         <v>46</v>
       </c>
       <c r="C44" s="20" t="s">
-        <v>241</v>
+        <v>210</v>
       </c>
       <c r="D44" s="23" t="s">
-        <v>205</v>
+        <v>175</v>
       </c>
       <c r="E44" s="23" t="s">
-        <v>206</v>
+        <v>176</v>
       </c>
       <c r="F44" s="18" t="s">
-        <v>229</v>
+        <v>198</v>
       </c>
       <c r="G44" s="18"/>
       <c r="H44" s="28"/>
@@ -2759,19 +2787,19 @@
         <v>47</v>
       </c>
       <c r="C45" s="20" t="s">
-        <v>193</v>
+        <v>163</v>
       </c>
       <c r="D45" s="23" t="s">
-        <v>189</v>
+        <v>159</v>
       </c>
       <c r="E45" s="23" t="s">
-        <v>107</v>
+        <v>78</v>
       </c>
       <c r="F45" s="18" t="s">
-        <v>226</v>
+        <v>195</v>
       </c>
       <c r="G45" s="27" t="s">
-        <v>191</v>
+        <v>161</v>
       </c>
       <c r="H45" s="28"/>
     </row>
@@ -2781,19 +2809,19 @@
         <v>48</v>
       </c>
       <c r="C46" s="20" t="s">
-        <v>194</v>
+        <v>164</v>
       </c>
       <c r="D46" s="23" t="s">
-        <v>190</v>
+        <v>160</v>
       </c>
       <c r="E46" s="23" t="s">
-        <v>108</v>
+        <v>79</v>
       </c>
       <c r="F46" s="18" t="s">
-        <v>226</v>
+        <v>195</v>
       </c>
       <c r="G46" s="27" t="s">
-        <v>192</v>
+        <v>162</v>
       </c>
       <c r="H46" s="28"/>
     </row>
@@ -2803,14 +2831,14 @@
         <v>49</v>
       </c>
       <c r="C47" s="19" t="s">
-        <v>212</v>
+        <v>182</v>
       </c>
       <c r="D47" s="24"/>
       <c r="E47" s="23" t="s">
-        <v>250</v>
+        <v>219</v>
       </c>
       <c r="F47" s="18" t="s">
-        <v>254</v>
+        <v>223</v>
       </c>
       <c r="G47" s="27"/>
       <c r="H47" s="28"/>
@@ -2821,14 +2849,14 @@
         <v>50</v>
       </c>
       <c r="C48" s="19" t="s">
-        <v>213</v>
+        <v>183</v>
       </c>
       <c r="D48" s="24"/>
       <c r="E48" s="23" t="s">
-        <v>251</v>
+        <v>220</v>
       </c>
       <c r="F48" s="18" t="s">
-        <v>254</v>
+        <v>223</v>
       </c>
       <c r="G48" s="27"/>
       <c r="H48" s="28"/>
@@ -2839,14 +2867,14 @@
         <v>51</v>
       </c>
       <c r="C49" s="19" t="s">
-        <v>214</v>
+        <v>184</v>
       </c>
       <c r="D49" s="24"/>
       <c r="E49" s="23" t="s">
-        <v>252</v>
+        <v>221</v>
       </c>
       <c r="F49" s="18" t="s">
-        <v>254</v>
+        <v>223</v>
       </c>
       <c r="G49" s="27"/>
       <c r="H49" s="28"/>
@@ -2857,14 +2885,14 @@
         <v>52</v>
       </c>
       <c r="C50" s="19" t="s">
-        <v>249</v>
+        <v>218</v>
       </c>
       <c r="D50" s="24"/>
       <c r="E50" s="23" t="s">
-        <v>253</v>
+        <v>222</v>
       </c>
       <c r="F50" s="18" t="s">
-        <v>254</v>
+        <v>223</v>
       </c>
       <c r="G50" s="27"/>
       <c r="H50" s="28"/>
@@ -2876,36 +2904,36 @@
       </c>
       <c r="C51" s="24"/>
       <c r="D51" s="24" t="s">
-        <v>220</v>
+        <v>189</v>
       </c>
       <c r="E51" s="23"/>
       <c r="F51" s="18"/>
       <c r="G51" s="27" t="s">
-        <v>221</v>
+        <v>190</v>
       </c>
       <c r="H51" s="28"/>
     </row>
     <row r="52" spans="1:8" ht="57.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="32" t="s">
-        <v>83</v>
+        <v>54</v>
       </c>
       <c r="B52" s="26">
         <v>1</v>
       </c>
       <c r="C52" s="24" t="s">
-        <v>162</v>
+        <v>133</v>
       </c>
       <c r="D52" s="24" t="s">
-        <v>161</v>
+        <v>132</v>
       </c>
       <c r="E52" s="24" t="s">
-        <v>109</v>
+        <v>80</v>
       </c>
       <c r="F52" s="18" t="s">
-        <v>229</v>
+        <v>198</v>
       </c>
       <c r="G52" s="18" t="s">
-        <v>244</v>
+        <v>213</v>
       </c>
       <c r="H52" s="28"/>
     </row>
@@ -2915,19 +2943,19 @@
         <v>2</v>
       </c>
       <c r="C53" s="24" t="s">
-        <v>163</v>
+        <v>134</v>
       </c>
       <c r="D53" s="24" t="s">
-        <v>207</v>
+        <v>177</v>
       </c>
       <c r="E53" s="24" t="s">
-        <v>110</v>
+        <v>81</v>
       </c>
       <c r="F53" s="18" t="s">
-        <v>229</v>
+        <v>198</v>
       </c>
       <c r="G53" s="18" t="s">
-        <v>222</v>
+        <v>191</v>
       </c>
       <c r="H53" s="28"/>
     </row>
@@ -2949,8 +2977,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2968,367 +2996,367 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" s="41" t="s">
-        <v>259</v>
+        <v>228</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>260</v>
+        <v>229</v>
       </c>
       <c r="C1" s="36" t="s">
-        <v>270</v>
+        <v>237</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" s="41"/>
       <c r="B2" s="6" t="s">
-        <v>17</v>
+        <v>257</v>
       </c>
       <c r="C2" s="36"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" s="41" t="s">
-        <v>60</v>
+        <v>33</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>70</v>
+        <v>261</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" s="41"/>
       <c r="B4" s="7" t="s">
-        <v>18</v>
+        <v>258</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" s="41"/>
       <c r="B5" s="6" t="s">
-        <v>19</v>
+        <v>259</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A6" s="41" t="s">
-        <v>258</v>
+        <v>227</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>28</v>
+        <v>262</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A7" s="41"/>
       <c r="B7" s="6" t="s">
-        <v>53</v>
+        <v>263</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A8" s="41" t="s">
-        <v>257</v>
+        <v>226</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>54</v>
+        <v>264</v>
       </c>
       <c r="C8" s="36" t="s">
-        <v>269</v>
+        <v>236</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A9" s="41"/>
       <c r="B9" s="6" t="s">
-        <v>55</v>
+        <v>265</v>
       </c>
       <c r="C9" s="36"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A10" s="31" t="s">
-        <v>256</v>
+        <v>225</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>56</v>
+        <v>266</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A11" s="40" t="s">
-        <v>255</v>
+        <v>224</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>57</v>
+        <v>267</v>
       </c>
       <c r="C11" s="36" t="s">
-        <v>271</v>
+        <v>238</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A12" s="40"/>
       <c r="B12" s="6" t="s">
-        <v>58</v>
+        <v>268</v>
       </c>
       <c r="C12" s="36"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A13" s="40" t="s">
-        <v>267</v>
+        <v>234</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="C13" s="36" t="s">
-        <v>268</v>
+        <v>235</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A14" s="40"/>
       <c r="B14" s="6" t="s">
-        <v>261</v>
+        <v>230</v>
       </c>
       <c r="C14" s="36"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A15" s="42" t="s">
-        <v>263</v>
+        <v>231</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>265</v>
+        <v>232</v>
       </c>
       <c r="C15" s="36" t="s">
-        <v>266</v>
+        <v>233</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A16" s="43"/>
       <c r="B16" s="6" t="s">
-        <v>262</v>
+        <v>269</v>
       </c>
       <c r="C16" s="44"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A17" s="40" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>20</v>
+        <v>239</v>
       </c>
       <c r="C17" s="37" t="s">
-        <v>64</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A18" s="40"/>
       <c r="B18" s="5" t="s">
-        <v>21</v>
+        <v>240</v>
       </c>
       <c r="C18" s="38"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A19" s="40"/>
       <c r="B19" s="5" t="s">
-        <v>22</v>
+        <v>242</v>
       </c>
       <c r="C19" s="38"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A20" s="40"/>
       <c r="B20" s="5" t="s">
-        <v>23</v>
+        <v>243</v>
       </c>
       <c r="C20" s="38"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A21" s="40"/>
       <c r="B21" s="5" t="s">
-        <v>24</v>
+        <v>244</v>
       </c>
       <c r="C21" s="38"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A22" s="40"/>
       <c r="B22" s="5" t="s">
-        <v>25</v>
+        <v>245</v>
       </c>
       <c r="C22" s="38"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A23" s="40"/>
       <c r="B23" s="5" t="s">
-        <v>26</v>
+        <v>246</v>
       </c>
       <c r="C23" s="38"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A24" s="40"/>
       <c r="B24" s="5" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="C24" s="38"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A25" s="40" t="s">
-        <v>61</v>
+        <v>247</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>31</v>
+        <v>248</v>
       </c>
       <c r="C25" s="38"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A26" s="40"/>
       <c r="B26" s="6" t="s">
-        <v>34</v>
+        <v>249</v>
       </c>
       <c r="C26" s="38"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A27" s="40"/>
       <c r="B27" s="6" t="s">
-        <v>37</v>
+        <v>250</v>
       </c>
       <c r="C27" s="38"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A28" s="40"/>
       <c r="B28" s="6" t="s">
-        <v>40</v>
+        <v>251</v>
       </c>
       <c r="C28" s="38"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A29" s="40"/>
       <c r="B29" s="6" t="s">
-        <v>43</v>
+        <v>252</v>
       </c>
       <c r="C29" s="38"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A30" s="40"/>
       <c r="B30" s="6" t="s">
-        <v>46</v>
+        <v>253</v>
       </c>
       <c r="C30" s="38"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A31" s="40"/>
       <c r="B31" s="6" t="s">
-        <v>49</v>
+        <v>254</v>
       </c>
       <c r="C31" s="38"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A32" s="40"/>
       <c r="B32" s="6" t="s">
-        <v>52</v>
+        <v>255</v>
       </c>
       <c r="C32" s="38"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A33" s="40" t="s">
-        <v>62</v>
+        <v>34</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>30</v>
+        <v>256</v>
       </c>
       <c r="C33" s="38"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A34" s="40"/>
       <c r="B34" s="7" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="C34" s="38"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A35" s="40"/>
       <c r="B35" s="7" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="C35" s="38"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A36" s="40"/>
       <c r="B36" s="7" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="C36" s="38"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A37" s="40"/>
       <c r="B37" s="7" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="C37" s="38"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A38" s="40"/>
       <c r="B38" s="7" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="C38" s="38"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A39" s="40"/>
       <c r="B39" s="7" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="C39" s="38"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A40" s="40"/>
       <c r="B40" s="7" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="C40" s="38"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A41" s="40" t="s">
-        <v>63</v>
+        <v>35</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="C41" s="38"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A42" s="40"/>
       <c r="B42" s="8" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="C42" s="38"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A43" s="40"/>
       <c r="B43" s="8" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="C43" s="38"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A44" s="40"/>
       <c r="B44" s="8" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="C44" s="38"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A45" s="40"/>
       <c r="B45" s="8" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="C45" s="38"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A46" s="40"/>
       <c r="B46" s="8" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="C46" s="38"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A47" s="40"/>
       <c r="B47" s="8" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="C47" s="38"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A48" s="40"/>
       <c r="B48" s="8" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="C48" s="39"/>
     </row>
@@ -3337,6 +3365,7 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="C11:C12"/>
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="C17:C48"/>
@@ -3353,7 +3382,6 @@
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="C15:C16"/>
     <mergeCell ref="C13:C14"/>
-    <mergeCell ref="C11:C12"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update factory test including standy_mode, shutdown, usb_LED turn off and paly_volume update.
</commit_message>
<xml_diff>
--- a/R1_test_command_list_tag1.7PTE.xlsx
+++ b/R1_test_command_list_tag1.7PTE.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="275">
   <si>
     <t>./inventory.sh</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -160,10 +160,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>adb shell /etc/factory-test/r1/enter_factory_mode.sh</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>adb shell /etc/factory-test/r1/exit_factory_mode.sh</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -172,10 +168,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>adb shell /etc/factory-test/r1/inventory.sh</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>adb shell /etc/factory-test/r1/set_shutdown.sh</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -193,10 +185,6 @@
   </si>
   <si>
     <t>loop_back_mode.sh</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>set_standby_mode.sh</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -420,10 +408,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>adb shell /etc/factory-test/r1/get_bat_name.sh</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>bq40z50-R2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -452,10 +436,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>adb shell /etc/factory-test/r1/set_bat_shutdown.sh</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>current: -487 mA</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -468,10 +448,6 @@
   </si>
   <si>
     <t>get_bat_temp.sh</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>adb shell /etc/factory-test/r1/play_file.sh song.wav</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -680,9 +656,6 @@
     <t>pull_file.bat /data/factory-test/mic-4ch.wav</t>
   </si>
   <si>
-    <t>Added in 1.1.9 .Only resets volume so far</t>
-  </si>
-  <si>
     <t>Set_ANC_enable.sh</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -839,10 +812,6 @@
   </si>
   <si>
     <t>Connect to WiFi</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Set_Amplifier_poweron.sh</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1132,10 +1101,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>adb shell /etc/factory-test/r1/set_volume.sh 0.3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>adb shell /etc/factory-test/r1/factory_reset.sh</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1164,7 +1129,71 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>adb shell /etc/factory-test/r1/enter_factory_mode.sh</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>adb shell /etc/factory-test/r1/get_bat_name.sh</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>adb shell /etc/factory-test/r1/inventory.sh</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>adb shell /etc/factory-test/r1/set_bat_shutdown.sh</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Set_Amplifier_poweron.sh</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>set_standby_mode.sh</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(need to test)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Miss command,  temporarily do not support this fcuntion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>adb shell /etc/factory-test/r1/set_standby_mode.sh</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>set_usbled_off.sh</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>adb shell /etc/factory-test/r1/get_bt_name.sh</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>adb shell /etc/factory-test/r1/set_usbled_off.sh</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>set usb breath led off</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Added in 2.1.3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>deleted in 2.1.3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>adb shell /etc/factory-test/r1/play_file.sh song.wav  sounds_value</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Changed in 2.1.3, please add a sound value parameter in the end of this command,  and to set the volume value</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1484,6 +1513,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1492,24 +1539,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1815,10 +1844,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H58"/>
+  <dimension ref="A1:H59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+    <sheetView tabSelected="1" topLeftCell="B28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
@@ -1836,7 +1865,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>15</v>
@@ -1851,33 +1880,33 @@
         <v>14</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G1" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" s="15" t="s">
         <v>50</v>
-      </c>
-      <c r="H1" s="15" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B2" s="24">
         <v>1</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E2" s="16" t="s">
         <v>9</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="G2" s="17"/>
       <c r="H2" s="27"/>
@@ -1888,19 +1917,19 @@
         <v>2</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="F3" s="17" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="G3" s="17" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="H3" s="27"/>
     </row>
@@ -1913,16 +1942,16 @@
         <v>2</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>38</v>
+        <v>258</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="G4" s="17" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="H4" s="27"/>
     </row>
@@ -1935,16 +1964,16 @@
         <v>3</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="G5" s="17" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="H5" s="27"/>
     </row>
@@ -1954,19 +1983,19 @@
         <v>5</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E6" s="17" t="s">
         <v>7</v>
       </c>
       <c r="F6" s="17" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="G6" s="17" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="H6" s="27"/>
     </row>
@@ -1985,7 +2014,7 @@
         <v>11</v>
       </c>
       <c r="F7" s="17" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="G7" s="17"/>
       <c r="H7" s="27"/>
@@ -1995,13 +2024,13 @@
       <c r="B8" s="24"/>
       <c r="C8" s="19"/>
       <c r="D8" s="17" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="G8" s="17"/>
       <c r="H8" s="27"/>
@@ -2012,19 +2041,19 @@
         <v>7</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="G9" s="17" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="H9" s="27"/>
     </row>
@@ -2037,16 +2066,16 @@
         <v>0</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>41</v>
+        <v>260</v>
       </c>
       <c r="E10" s="17" t="s">
         <v>6</v>
       </c>
       <c r="F10" s="17" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="G10" s="17" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="H10" s="27"/>
     </row>
@@ -2056,19 +2085,19 @@
         <v>9</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="E11" s="16" t="s">
         <v>10</v>
       </c>
       <c r="F11" s="17" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="G11" s="17" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="H11" s="27"/>
     </row>
@@ -2078,19 +2107,19 @@
         <v>10</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="F12" s="17" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="G12" s="28" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="H12" s="27"/>
     </row>
@@ -2100,16 +2129,16 @@
         <v>11</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="E13" s="17" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="F13" s="17" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="G13" s="17"/>
       <c r="H13" s="27"/>
@@ -2120,16 +2149,16 @@
         <v>12</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="E14" s="17" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="F14" s="17" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="G14" s="17"/>
       <c r="H14" s="27"/>
@@ -2140,16 +2169,16 @@
         <v>13</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="E15" s="17" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="F15" s="17" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="G15" s="17"/>
       <c r="H15" s="27"/>
@@ -2163,16 +2192,16 @@
         <v>1</v>
       </c>
       <c r="D16" s="23" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E16" s="17" t="s">
         <v>5</v>
       </c>
       <c r="F16" s="17" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="G16" s="17" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H16" s="27"/>
     </row>
@@ -2182,56 +2211,56 @@
         <v>15</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="D17" s="23" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E17" s="16" t="s">
         <v>8</v>
       </c>
       <c r="F17" s="16"/>
       <c r="G17" s="17" t="s">
-        <v>188</v>
-      </c>
-      <c r="H17" s="27"/>
+        <v>181</v>
+      </c>
+      <c r="H17" s="11"/>
     </row>
     <row r="18" spans="1:8" ht="140" x14ac:dyDescent="0.25">
       <c r="A18" s="33"/>
       <c r="B18" s="24">
         <v>16</v>
       </c>
-      <c r="C18" s="19" t="s">
-        <v>96</v>
-      </c>
-      <c r="D18" s="23" t="s">
-        <v>259</v>
-      </c>
+      <c r="C18" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="D18" s="23"/>
       <c r="E18" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="F18" s="17" t="s">
-        <v>172</v>
+        <v>67</v>
+      </c>
+      <c r="F18" s="29" t="s">
+        <v>265</v>
       </c>
       <c r="G18" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="H18" s="27"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+      <c r="H18" s="11" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="37" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="33"/>
       <c r="B19" s="24">
         <v>17</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D19" s="23"/>
       <c r="E19" s="16" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F19" s="29" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="G19" s="17"/>
       <c r="H19" s="11"/>
@@ -2242,17 +2271,17 @@
         <v>18</v>
       </c>
       <c r="C20" s="19" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D20" s="23" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="E20" s="22" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F20" s="17"/>
       <c r="G20" s="17" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="H20" s="27"/>
     </row>
@@ -2262,17 +2291,17 @@
         <v>19</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D21" s="23" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="E21" s="22" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F21" s="17"/>
       <c r="G21" s="17" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="H21" s="27"/>
     </row>
@@ -2282,23 +2311,21 @@
         <v>20</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="D22" s="23" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="E22" s="16" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F22" s="22" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="G22" s="17" t="s">
-        <v>182</v>
-      </c>
-      <c r="H22" s="27" t="s">
-        <v>163</v>
-      </c>
+        <v>175</v>
+      </c>
+      <c r="H22" s="27"/>
     </row>
     <row r="23" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="33"/>
@@ -2306,19 +2333,19 @@
         <v>21</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D23" s="23" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="E23" s="22" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F23" s="22" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="G23" s="17" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="H23" s="27"/>
     </row>
@@ -2328,19 +2355,19 @@
         <v>22</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D24" s="23" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="E24" s="22" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F24" s="17" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="G24" s="17" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="H24" s="27"/>
     </row>
@@ -2350,19 +2377,19 @@
         <v>23</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D25" s="23" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E25" s="22" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F25" s="17" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="G25" s="17" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="H25" s="11"/>
     </row>
@@ -2372,19 +2399,19 @@
         <v>24</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D26" s="23" t="s">
-        <v>106</v>
+        <v>259</v>
       </c>
       <c r="E26" s="22" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F26" s="17" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="G26" s="17" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="H26" s="11"/>
     </row>
@@ -2394,19 +2421,19 @@
         <v>25</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D27" s="23" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E27" s="22" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F27" s="17" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="G27" s="17" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="H27" s="11"/>
     </row>
@@ -2416,19 +2443,19 @@
         <v>26</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D28" s="23" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E28" s="22" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F28" s="17" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="G28" s="17" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="H28" s="11"/>
     </row>
@@ -2438,22 +2465,22 @@
         <v>27</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="D29" s="23" t="s">
-        <v>114</v>
+        <v>261</v>
       </c>
       <c r="E29" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="F29" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="G29" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="H29" s="10" t="s">
         <v>128</v>
-      </c>
-      <c r="F29" s="17" t="s">
-        <v>171</v>
-      </c>
-      <c r="G29" s="17" t="s">
-        <v>159</v>
-      </c>
-      <c r="H29" s="10" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2462,18 +2489,18 @@
         <v>28</v>
       </c>
       <c r="C30" s="22" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D30" s="23"/>
       <c r="E30" s="22" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F30" s="17" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="G30" s="17"/>
       <c r="H30" s="10" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2482,19 +2509,19 @@
         <v>29</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="D31" s="23" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="E31" s="22" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F31" s="17" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="G31" s="17" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="H31" s="27"/>
     </row>
@@ -2504,19 +2531,19 @@
         <v>31</v>
       </c>
       <c r="C32" s="19" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="D32" s="23" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="E32" s="22" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="F32" s="26" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="G32" s="17" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="H32" s="27"/>
     </row>
@@ -2526,19 +2553,19 @@
         <v>32</v>
       </c>
       <c r="C33" s="19" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D33" s="23" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="E33" s="22" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="F33" s="26" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="G33" s="17" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="H33" s="27"/>
     </row>
@@ -2548,19 +2575,19 @@
         <v>33</v>
       </c>
       <c r="C34" s="19" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="D34" s="23" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="E34" s="22" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F34" s="17" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="G34" s="17" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="H34" s="27"/>
     </row>
@@ -2570,36 +2597,38 @@
         <v>34</v>
       </c>
       <c r="C35" s="19" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="D35" s="23" t="s">
-        <v>119</v>
+        <v>273</v>
       </c>
       <c r="E35" s="22" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F35" s="22" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="G35" s="17" t="s">
-        <v>186</v>
-      </c>
-      <c r="H35" s="27"/>
-    </row>
-    <row r="36" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+      <c r="H35" s="10" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="33"/>
       <c r="B36" s="24">
         <v>35</v>
       </c>
       <c r="C36" s="22" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D36" s="23"/>
       <c r="E36" s="22" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F36" s="29" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="G36" s="17"/>
       <c r="H36" s="11"/>
@@ -2610,19 +2639,19 @@
         <v>36</v>
       </c>
       <c r="C37" s="19" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="D37" s="23" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
       <c r="E37" s="22" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F37" s="17" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="G37" s="26" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="H37" s="27"/>
     </row>
@@ -2632,36 +2661,38 @@
         <v>37</v>
       </c>
       <c r="C38" s="19" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="D38" s="23" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="E38" s="22" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F38" s="17" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="G38" s="26" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="H38" s="27"/>
     </row>
-    <row r="39" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="33"/>
       <c r="B39" s="24">
         <v>38</v>
       </c>
       <c r="C39" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="D39" s="23"/>
+        <v>263</v>
+      </c>
+      <c r="D39" s="23" t="s">
+        <v>266</v>
+      </c>
       <c r="E39" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="F39" s="29" t="s">
-        <v>122</v>
+        <v>73</v>
+      </c>
+      <c r="F39" s="22" t="s">
+        <v>264</v>
       </c>
       <c r="G39" s="17"/>
       <c r="H39" s="11"/>
@@ -2672,19 +2703,19 @@
         <v>39</v>
       </c>
       <c r="C40" s="19" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D40" s="23" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="E40" s="22" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F40" s="17" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="G40" s="17" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="H40" s="11"/>
     </row>
@@ -2694,19 +2725,19 @@
         <v>40</v>
       </c>
       <c r="C41" s="19" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="D41" s="23" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="E41" s="22" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="F41" s="22" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="G41" s="17" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="H41" s="11"/>
     </row>
@@ -2716,18 +2747,18 @@
         <v>41</v>
       </c>
       <c r="C42" s="20" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D42" s="22"/>
       <c r="E42" s="22" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F42" s="29" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="G42" s="17"/>
       <c r="H42" s="10" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2736,16 +2767,16 @@
         <v>45</v>
       </c>
       <c r="C43" s="19" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="D43" s="22" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="E43" s="22" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="F43" s="17" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="G43" s="17"/>
       <c r="H43" s="27"/>
@@ -2756,16 +2787,16 @@
         <v>46</v>
       </c>
       <c r="C44" s="19" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="D44" s="22" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="E44" s="22" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="F44" s="17" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="G44" s="17"/>
       <c r="H44" s="27"/>
@@ -2776,19 +2807,19 @@
         <v>47</v>
       </c>
       <c r="C45" s="19" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="D45" s="22" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="E45" s="22" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F45" s="17" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="G45" s="26" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="H45" s="27"/>
     </row>
@@ -2798,56 +2829,56 @@
         <v>48</v>
       </c>
       <c r="C46" s="19" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D46" s="22" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="E46" s="22" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F46" s="17" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="G46" s="26" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="H46" s="27"/>
     </row>
     <row r="47" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="33"/>
-      <c r="B47" s="24">
-        <v>49</v>
-      </c>
+      <c r="B47" s="24"/>
       <c r="C47" s="18" t="s">
-        <v>266</v>
-      </c>
-      <c r="D47" s="23" t="s">
         <v>267</v>
       </c>
+      <c r="D47" s="22" t="s">
+        <v>269</v>
+      </c>
       <c r="E47" s="22" t="s">
-        <v>192</v>
-      </c>
-      <c r="F47" s="17" t="s">
-        <v>196</v>
-      </c>
+        <v>270</v>
+      </c>
+      <c r="F47" s="17"/>
       <c r="G47" s="26"/>
-      <c r="H47" s="27"/>
+      <c r="H47" s="27" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="48" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="33"/>
       <c r="B48" s="24">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C48" s="18" t="s">
-        <v>164</v>
-      </c>
-      <c r="D48" s="23"/>
+        <v>257</v>
+      </c>
+      <c r="D48" s="23" t="s">
+        <v>268</v>
+      </c>
       <c r="E48" s="22" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="F48" s="17" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="G48" s="26"/>
       <c r="H48" s="27"/>
@@ -2855,17 +2886,17 @@
     <row r="49" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="33"/>
       <c r="B49" s="24">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C49" s="18" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="D49" s="23"/>
       <c r="E49" s="22" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="F49" s="17" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="G49" s="26"/>
       <c r="H49" s="27"/>
@@ -2873,90 +2904,108 @@
     <row r="50" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="33"/>
       <c r="B50" s="24">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C50" s="18" t="s">
-        <v>191</v>
+        <v>158</v>
       </c>
       <c r="D50" s="23"/>
       <c r="E50" s="22" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="F50" s="17" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="G50" s="26"/>
       <c r="H50" s="27"/>
     </row>
     <row r="51" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="34"/>
+      <c r="A51" s="33"/>
       <c r="B51" s="24">
+        <v>52</v>
+      </c>
+      <c r="C51" s="18" t="s">
+        <v>262</v>
+      </c>
+      <c r="D51" s="23"/>
+      <c r="E51" s="22" t="s">
+        <v>187</v>
+      </c>
+      <c r="F51" s="17" t="s">
+        <v>188</v>
+      </c>
+      <c r="G51" s="26"/>
+      <c r="H51" s="27"/>
+    </row>
+    <row r="52" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="34"/>
+      <c r="B52" s="24">
         <v>53</v>
       </c>
-      <c r="C51" s="23"/>
-      <c r="D51" s="23" t="s">
-        <v>167</v>
-      </c>
-      <c r="E51" s="22"/>
-      <c r="F51" s="17"/>
-      <c r="G51" s="26" t="s">
+      <c r="C52" s="23"/>
+      <c r="D52" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="E52" s="22"/>
+      <c r="F52" s="17"/>
+      <c r="G52" s="26" t="s">
+        <v>161</v>
+      </c>
+      <c r="H52" s="27"/>
+    </row>
+    <row r="53" spans="1:8" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="B53" s="25">
+        <v>1</v>
+      </c>
+      <c r="C53" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="D53" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="E53" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="F53" s="17" t="s">
         <v>168</v>
       </c>
-      <c r="H51" s="27"/>
-    </row>
-    <row r="52" spans="1:8" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="31" t="s">
-        <v>54</v>
-      </c>
-      <c r="B52" s="25">
-        <v>1</v>
-      </c>
-      <c r="C52" s="23" t="s">
-        <v>125</v>
-      </c>
-      <c r="D52" s="23" t="s">
-        <v>124</v>
-      </c>
-      <c r="E52" s="23" t="s">
-        <v>80</v>
-      </c>
-      <c r="F52" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="G52" s="17" t="s">
-        <v>187</v>
-      </c>
-      <c r="H52" s="27"/>
-    </row>
-    <row r="53" spans="1:8" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="31"/>
-      <c r="B53" s="25">
+      <c r="G53" s="17" t="s">
+        <v>180</v>
+      </c>
+      <c r="H53" s="27"/>
+    </row>
+    <row r="54" spans="1:8" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="31"/>
+      <c r="B54" s="25">
         <v>2</v>
       </c>
-      <c r="C53" s="23" t="s">
-        <v>126</v>
-      </c>
-      <c r="D53" s="23" t="s">
+      <c r="C54" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="D54" s="23" t="s">
+        <v>156</v>
+      </c>
+      <c r="E54" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="F54" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="G54" s="17" t="s">
         <v>162</v>
       </c>
-      <c r="E53" s="23" t="s">
-        <v>81</v>
-      </c>
-      <c r="F53" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="G53" s="17" t="s">
-        <v>169</v>
-      </c>
-      <c r="H53" s="27"/>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D58"/>
+      <c r="H54" s="27"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D59"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="A2:A51"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="A2:A52"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2986,393 +3035,393 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="40" t="s">
+        <v>193</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="C1" s="35" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="40"/>
+      <c r="B2" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="C2" s="35"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="40"/>
+      <c r="B4" s="7" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="40"/>
+      <c r="B5" s="6" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="40" t="s">
+        <v>192</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="40"/>
+      <c r="B7" s="6" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="40" t="s">
+        <v>191</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="C8" s="35" t="s">
         <v>201</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>202</v>
-      </c>
-      <c r="C1" s="39" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="38"/>
-      <c r="B2" s="6" t="s">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="40"/>
+      <c r="B9" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="C2" s="39"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="38" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="38"/>
-      <c r="B4" s="7" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="38"/>
-      <c r="B5" s="6" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="38" t="s">
-        <v>200</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="38"/>
-      <c r="B7" s="6" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="38" t="s">
-        <v>199</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>237</v>
-      </c>
-      <c r="C8" s="39" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="38"/>
-      <c r="B9" s="6" t="s">
-        <v>238</v>
-      </c>
-      <c r="C9" s="39"/>
+      <c r="C9" s="35"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="30" t="s">
+        <v>190</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="41" t="s">
+        <v>189</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="C11" s="35" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="41"/>
+      <c r="B12" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="C12" s="35"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="41" t="s">
+        <v>199</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="C13" s="35" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="41"/>
+      <c r="B14" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="C14" s="35"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="42" t="s">
+        <v>196</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="C15" s="35" t="s">
         <v>198</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="35" t="s">
-        <v>197</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>240</v>
-      </c>
-      <c r="C11" s="39" t="s">
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="43"/>
+      <c r="B16" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="C16" s="39"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="C17" s="36" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="41"/>
+      <c r="B18" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="C18" s="37"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="41"/>
+      <c r="B19" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="C19" s="37"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="41"/>
+      <c r="B20" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C20" s="37"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="41"/>
+      <c r="B21" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="C21" s="37"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="41"/>
+      <c r="B22" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C22" s="37"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="41"/>
+      <c r="B23" s="5" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="35"/>
-      <c r="B12" s="6" t="s">
-        <v>241</v>
-      </c>
-      <c r="C12" s="39"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="35" t="s">
-        <v>207</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="C13" s="39" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="35"/>
-      <c r="B14" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="C14" s="39"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="36" t="s">
-        <v>204</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>205</v>
-      </c>
-      <c r="C15" s="39" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="37"/>
-      <c r="B16" s="6" t="s">
-        <v>242</v>
-      </c>
-      <c r="C16" s="43"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="35" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="C17" s="40" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="35"/>
-      <c r="B18" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="C18" s="41"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="35"/>
-      <c r="B19" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="C19" s="41"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="35"/>
-      <c r="B20" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="C20" s="41"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="35"/>
-      <c r="B21" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="C21" s="41"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="35"/>
-      <c r="B22" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="C22" s="41"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="35"/>
-      <c r="B23" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="C23" s="41"/>
+      <c r="C23" s="37"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="35"/>
+      <c r="A24" s="41"/>
       <c r="B24" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="41"/>
+      <c r="C24" s="37"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="35" t="s">
+      <c r="A25" s="41" t="s">
+        <v>212</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="C25" s="37"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="41"/>
+      <c r="B26" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="C26" s="37"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="41"/>
+      <c r="B27" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="C27" s="37"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="41"/>
+      <c r="B28" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="C28" s="37"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="41"/>
+      <c r="B29" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="C29" s="37"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="41"/>
+      <c r="B30" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="C30" s="37"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="41"/>
+      <c r="B31" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="C31" s="37"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="41"/>
+      <c r="B32" s="6" t="s">
         <v>220</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="C32" s="37"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="B33" s="7" t="s">
         <v>221</v>
       </c>
-      <c r="C25" s="41"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="35"/>
-      <c r="B26" s="6" t="s">
-        <v>222</v>
-      </c>
-      <c r="C26" s="41"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="35"/>
-      <c r="B27" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="C27" s="41"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="35"/>
-      <c r="B28" s="6" t="s">
-        <v>224</v>
-      </c>
-      <c r="C28" s="41"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="35"/>
-      <c r="B29" s="6" t="s">
-        <v>225</v>
-      </c>
-      <c r="C29" s="41"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="35"/>
-      <c r="B30" s="6" t="s">
-        <v>226</v>
-      </c>
-      <c r="C30" s="41"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="35"/>
-      <c r="B31" s="6" t="s">
-        <v>227</v>
-      </c>
-      <c r="C31" s="41"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="35"/>
-      <c r="B32" s="6" t="s">
-        <v>228</v>
-      </c>
-      <c r="C32" s="41"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="35" t="s">
-        <v>34</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>229</v>
-      </c>
-      <c r="C33" s="41"/>
+      <c r="C33" s="37"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="35"/>
+      <c r="A34" s="41"/>
       <c r="B34" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C34" s="41"/>
+      <c r="C34" s="37"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="35"/>
+      <c r="A35" s="41"/>
       <c r="B35" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C35" s="41"/>
+      <c r="C35" s="37"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="35"/>
+      <c r="A36" s="41"/>
       <c r="B36" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C36" s="41"/>
+      <c r="C36" s="37"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="35"/>
+      <c r="A37" s="41"/>
       <c r="B37" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C37" s="41"/>
+      <c r="C37" s="37"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="35"/>
+      <c r="A38" s="41"/>
       <c r="B38" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C38" s="41"/>
+      <c r="C38" s="37"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="35"/>
+      <c r="A39" s="41"/>
       <c r="B39" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C39" s="41"/>
+      <c r="C39" s="37"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="35"/>
+      <c r="A40" s="41"/>
       <c r="B40" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C40" s="41"/>
+      <c r="C40" s="37"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="35" t="s">
+      <c r="A41" s="41" t="s">
         <v>35</v>
       </c>
       <c r="B41" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C41" s="41"/>
+      <c r="C41" s="37"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="35"/>
+      <c r="A42" s="41"/>
       <c r="B42" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C42" s="41"/>
+      <c r="C42" s="37"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="35"/>
+      <c r="A43" s="41"/>
       <c r="B43" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C43" s="41"/>
+      <c r="C43" s="37"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="35"/>
+      <c r="A44" s="41"/>
       <c r="B44" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C44" s="41"/>
+      <c r="C44" s="37"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="35"/>
+      <c r="A45" s="41"/>
       <c r="B45" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C45" s="41"/>
+      <c r="C45" s="37"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="35"/>
+      <c r="A46" s="41"/>
       <c r="B46" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C46" s="41"/>
+      <c r="C46" s="37"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="35"/>
+      <c r="A47" s="41"/>
       <c r="B47" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C47" s="41"/>
+      <c r="C47" s="37"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="35"/>
+      <c r="A48" s="41"/>
       <c r="B48" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C48" s="42"/>
+      <c r="C48" s="38"/>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A25:A32"/>
+    <mergeCell ref="A33:A40"/>
+    <mergeCell ref="A41:A48"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A17:A24"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A6:A7"/>
     <mergeCell ref="C13:C14"/>
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="C17:C48"/>
     <mergeCell ref="C15:C16"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A25:A32"/>
-    <mergeCell ref="A33:A40"/>
-    <mergeCell ref="A41:A48"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A17:A24"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update the default valume value
Signed-off-by: Jerry <348428118@qq.com>
</commit_message>
<xml_diff>
--- a/R1_test_command_list_tag1.7PTE.xlsx
+++ b/R1_test_command_list_tag1.7PTE.xlsx
@@ -761,25 +761,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>D:\Fancy.Liu\Tool\Android&gt;adb shell /etc/factory-test/r1/play_file.sh /etc/factory-test/r1/song.wav
-[ GST ] ----------------- set config path: /data/FLOWDSP/default_config.flw -------------
-Setting pipeline to PAUSED ...
-Failed to symlink /home/root/.config/pulse/aa6df7886f3448b2aa86718040c7c0b5-runtime to /tmp/pulse-PKdhtXMmr18n: Read-only file system
-[ GST ] ----------------- gst flowdsp plugin starts -------------
-Pipeline is PREROLLING ...
-ERROR: from element /GstPipeline:pipeline0/GstWavParse:wavparse0: Internal data stream error.
-Additional debug info:
-../../../gst-plugins-good-1.14.4/gst/wavparse/gstwavparse.c(2293): gst_wavparse_loop (): /GstPipeline:pipeline0/GstWavParse:wavparse0:
-streaming stopped, reason not-negotiated (-4)
-ERROR: pipeline doesn't want to preroll.
-Setting pipeline to NULL ...
-[ GST ] ----------------- stopped -------------
-Caught SIGSEGV
-exec gdb failed: No such file or directory
-Spinning.  Please run 'gdb gst-launch-1.0 3789' to continue debugging, Ctrl-C to quit, or Ctrl-\ to dump core.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>D:\Fancy.Liu\Tool\Android&gt;adb push song.wav /etc/factory-test/r1
 [100%] /etc/factory-test/r1/song.wav</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1121,10 +1102,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>play_file.sh &lt;file_name&gt;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>get_BT_name.sh</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1193,7 +1170,30 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Changed in 2.1.3, please add a sound value parameter in the end of this command,  and to set the volume value</t>
+    <t xml:space="preserve">Changed in 2.1.3, please add a sound value parameter (from 0 - 10, min - max) in the end of this command,  and to set the volume value </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D:\Fancy.Liu\Tool\Android&gt;adb shell /etc/factory-testE35:G35tory-test/r1/song.wav
+[ GST ] ----------------- set config path: /data/FLOWDSP/default_config.flw -------------
+Setting pipeline to PAUSED ...
+Failed to symlink /home/root/.config/pulse/aa6df7886f3448b2aa86718040c7c0b5-runtime to /tmp/pulse-PKdhtXMmr18n: Read-only file system
+[ GST ] ----------------- gst flowdsp plugin starts -------------
+Pipeline is PREROLLING ...
+ERROR: from element /GstPipeline:pipeline0/GstWavParse:wavparse0: Internal data stream error.
+Additional debug info:
+../../../gst-plugins-good-1.14.4/gst/wavparse/gstwavparse.c(2293): gst_wavparse_loop (): /GstPipeline:pipeline0/GstWavParse:wavparse0:
+streaming stopped, reason not-negotiated (-4)
+ERROR: pipeline doesn't want to preroll.
+Setting pipeline to NULL ...
+[ GST ] ----------------- stopped -------------
+Caught SIGSEGV
+exec gdb failed: No such file or directory
+Spinning.  Please run 'gdb gst-launch-1.0 3789' to continue debugging, Ctrl-C to quit, or Ctrl-\ to dump core.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>play_file.sh &lt;file_name&gt;  &lt;sound_value&gt;</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1846,8 +1846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E38" activeCellId="1" sqref="C35 E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
@@ -1923,13 +1923,13 @@
         <v>82</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F3" s="17" t="s">
         <v>164</v>
       </c>
       <c r="G3" s="17" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H3" s="27"/>
     </row>
@@ -1942,7 +1942,7 @@
         <v>2</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E4" s="17" t="s">
         <v>48</v>
@@ -2066,7 +2066,7 @@
         <v>0</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E10" s="17" t="s">
         <v>6</v>
@@ -2088,7 +2088,7 @@
         <v>89</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E11" s="16" t="s">
         <v>10</v>
@@ -2110,7 +2110,7 @@
         <v>90</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E12" s="17" t="s">
         <v>134</v>
@@ -2132,10 +2132,10 @@
         <v>135</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E13" s="17" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F13" s="17" t="s">
         <v>165</v>
@@ -2152,7 +2152,7 @@
         <v>159</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E14" s="17" t="s">
         <v>124</v>
@@ -2169,10 +2169,10 @@
         <v>13</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E15" s="17" t="s">
         <v>125</v>
@@ -2211,7 +2211,7 @@
         <v>15</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D17" s="23" t="s">
         <v>83</v>
@@ -2221,7 +2221,7 @@
       </c>
       <c r="F17" s="16"/>
       <c r="G17" s="17" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H17" s="11"/>
     </row>
@@ -2238,13 +2238,13 @@
         <v>67</v>
       </c>
       <c r="F18" s="29" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="G18" s="17" t="s">
         <v>92</v>
       </c>
       <c r="H18" s="11" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="37" customHeight="1" x14ac:dyDescent="0.25">
@@ -2274,7 +2274,7 @@
         <v>96</v>
       </c>
       <c r="D20" s="23" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E20" s="22" t="s">
         <v>57</v>
@@ -2314,7 +2314,7 @@
         <v>137</v>
       </c>
       <c r="D22" s="23" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E22" s="16" t="s">
         <v>68</v>
@@ -2358,7 +2358,7 @@
         <v>99</v>
       </c>
       <c r="D24" s="23" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E24" s="22" t="s">
         <v>58</v>
@@ -2402,7 +2402,7 @@
         <v>104</v>
       </c>
       <c r="D26" s="23" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E26" s="22" t="s">
         <v>60</v>
@@ -2424,7 +2424,7 @@
         <v>106</v>
       </c>
       <c r="D27" s="23" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E27" s="22" t="s">
         <v>61</v>
@@ -2468,7 +2468,7 @@
         <v>138</v>
       </c>
       <c r="D29" s="23" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="E29" s="22" t="s">
         <v>122</v>
@@ -2512,7 +2512,7 @@
         <v>111</v>
       </c>
       <c r="D31" s="23" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E31" s="22" t="s">
         <v>63</v>
@@ -2556,7 +2556,7 @@
         <v>152</v>
       </c>
       <c r="D33" s="23" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E33" s="22" t="s">
         <v>127</v>
@@ -2578,7 +2578,7 @@
         <v>113</v>
       </c>
       <c r="D34" s="23" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E34" s="22" t="s">
         <v>64</v>
@@ -2596,23 +2596,23 @@
       <c r="B35" s="24">
         <v>34</v>
       </c>
-      <c r="C35" s="19" t="s">
-        <v>256</v>
+      <c r="C35" s="10" t="s">
+        <v>274</v>
       </c>
       <c r="D35" s="23" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E35" s="22" t="s">
         <v>43</v>
       </c>
       <c r="F35" s="22" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G35" s="17" t="s">
-        <v>179</v>
+        <v>273</v>
       </c>
       <c r="H35" s="10" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -2642,7 +2642,7 @@
         <v>140</v>
       </c>
       <c r="D37" s="23" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E37" s="22" t="s">
         <v>72</v>
@@ -2683,16 +2683,16 @@
         <v>38</v>
       </c>
       <c r="C39" s="22" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D39" s="23" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E39" s="22" t="s">
         <v>73</v>
       </c>
       <c r="F39" s="22" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="G39" s="17"/>
       <c r="H39" s="11"/>
@@ -2706,7 +2706,7 @@
         <v>45</v>
       </c>
       <c r="D40" s="23" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E40" s="22" t="s">
         <v>74</v>
@@ -2737,7 +2737,7 @@
         <v>171</v>
       </c>
       <c r="G41" s="17" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H41" s="11"/>
     </row>
@@ -2770,7 +2770,7 @@
         <v>177</v>
       </c>
       <c r="D43" s="22" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E43" s="22" t="s">
         <v>154</v>
@@ -2790,7 +2790,7 @@
         <v>178</v>
       </c>
       <c r="D44" s="22" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E44" s="22" t="s">
         <v>155</v>
@@ -2832,7 +2832,7 @@
         <v>145</v>
       </c>
       <c r="D46" s="22" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E46" s="22" t="s">
         <v>76</v>
@@ -2849,18 +2849,18 @@
       <c r="A47" s="33"/>
       <c r="B47" s="24"/>
       <c r="C47" s="18" t="s">
+        <v>265</v>
+      </c>
+      <c r="D47" s="22" t="s">
         <v>267</v>
       </c>
-      <c r="D47" s="22" t="s">
-        <v>269</v>
-      </c>
       <c r="E47" s="22" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F47" s="17"/>
       <c r="G47" s="26"/>
       <c r="H47" s="27" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2869,16 +2869,16 @@
         <v>49</v>
       </c>
       <c r="C48" s="18" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D48" s="23" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="E48" s="22" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F48" s="17" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G48" s="26"/>
       <c r="H48" s="27"/>
@@ -2893,10 +2893,10 @@
       </c>
       <c r="D49" s="23"/>
       <c r="E49" s="22" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F49" s="17" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G49" s="26"/>
       <c r="H49" s="27"/>
@@ -2911,10 +2911,10 @@
       </c>
       <c r="D50" s="23"/>
       <c r="E50" s="22" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F50" s="17" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G50" s="26"/>
       <c r="H50" s="27"/>
@@ -2925,14 +2925,14 @@
         <v>52</v>
       </c>
       <c r="C51" s="18" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D51" s="23"/>
       <c r="E51" s="22" t="s">
+        <v>186</v>
+      </c>
+      <c r="F51" s="17" t="s">
         <v>187</v>
-      </c>
-      <c r="F51" s="17" t="s">
-        <v>188</v>
       </c>
       <c r="G51" s="26"/>
       <c r="H51" s="27"/>
@@ -2973,7 +2973,7 @@
         <v>168</v>
       </c>
       <c r="G53" s="17" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H53" s="27"/>
     </row>
@@ -3036,19 +3036,19 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="40" t="s">
+        <v>192</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>194</v>
-      </c>
       <c r="C1" s="35" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="40"/>
       <c r="B2" s="6" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C2" s="35"/>
     </row>
@@ -3057,112 +3057,112 @@
         <v>33</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="40"/>
       <c r="B4" s="7" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="40"/>
       <c r="B5" s="6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="40" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="40"/>
       <c r="B7" s="6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="40" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C8" s="35" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="40"/>
       <c r="B9" s="6" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C9" s="35"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="30" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="41" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C11" s="35" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="41"/>
       <c r="B12" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C12" s="35"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="41" t="s">
+        <v>198</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="C13" s="35" t="s">
         <v>199</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>225</v>
-      </c>
-      <c r="C13" s="35" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="41"/>
       <c r="B14" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C14" s="35"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="42" t="s">
+        <v>195</v>
+      </c>
+      <c r="B15" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="C15" s="35" t="s">
         <v>197</v>
-      </c>
-      <c r="C15" s="35" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="43"/>
       <c r="B16" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C16" s="39"/>
     </row>
@@ -3171,7 +3171,7 @@
         <v>32</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C17" s="36" t="s">
         <v>36</v>
@@ -3180,42 +3180,42 @@
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="41"/>
       <c r="B18" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C18" s="37"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="41"/>
       <c r="B19" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C19" s="37"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="41"/>
       <c r="B20" s="5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C20" s="37"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="41"/>
       <c r="B21" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C21" s="37"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="41"/>
       <c r="B22" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C22" s="37"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="41"/>
       <c r="B23" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C23" s="37"/>
     </row>
@@ -3228,59 +3228,59 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="41" t="s">
+        <v>211</v>
+      </c>
+      <c r="B25" s="6" t="s">
         <v>212</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>213</v>
       </c>
       <c r="C25" s="37"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="41"/>
       <c r="B26" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C26" s="37"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="41"/>
       <c r="B27" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C27" s="37"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="41"/>
       <c r="B28" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C28" s="37"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="41"/>
       <c r="B29" s="6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C29" s="37"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="41"/>
       <c r="B30" s="6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C30" s="37"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="41"/>
       <c r="B31" s="6" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C31" s="37"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="41"/>
       <c r="B32" s="6" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C32" s="37"/>
     </row>
@@ -3289,7 +3289,7 @@
         <v>34</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C33" s="37"/>
     </row>

</xml_diff>